<commit_message>
Updates to README and Ontology
</commit_message>
<xml_diff>
--- a/ontology_cip_2015_10_26_short.xlsx
+++ b/ontology_cip_2015_10_26_short.xlsx
@@ -2725,18 +2725,12 @@
     <t>SHI= (NOPH / NOPS)</t>
   </si>
   <si>
-    <t>PltHrv_Ct_plot</t>
-  </si>
-  <si>
     <t>SHI</t>
   </si>
   <si>
     <t>Yield of total roots per hectar</t>
   </si>
   <si>
-    <t>PltEst_Ct_plot</t>
-  </si>
-  <si>
     <t>PltEst</t>
   </si>
   <si>
@@ -2968,15 +2962,6 @@
     <t>FlsTtC</t>
   </si>
   <si>
-    <t>PltRts_Ct_plot</t>
-  </si>
-  <si>
-    <t>PltCRt_Ct_plot</t>
-  </si>
-  <si>
-    <t>PltNCR_Ct_plot</t>
-  </si>
-  <si>
     <t>RtsFWt_Ms_g</t>
   </si>
   <si>
@@ -3067,9 +3052,6 @@
     <t>Counting plants/vines planted.</t>
   </si>
   <si>
-    <t>PltPld_Ct_plot</t>
-  </si>
-  <si>
     <t>VirSm1_Et_1to9</t>
   </si>
   <si>
@@ -3143,6 +3125,24 @@
   </si>
   <si>
     <t>RtsSpA_Et_1to9</t>
+  </si>
+  <si>
+    <t>PltPld_Ct_plplot</t>
+  </si>
+  <si>
+    <t>PltEst_Ct_plplot</t>
+  </si>
+  <si>
+    <t>PltHrv_Ct_plplot</t>
+  </si>
+  <si>
+    <t>PltRts_Ct_plplot</t>
+  </si>
+  <si>
+    <t>PltCRt_Ct_plplot</t>
+  </si>
+  <si>
+    <t>PltNCR_Ct_plplot</t>
   </si>
 </sst>
 </file>
@@ -5518,11 +5518,11 @@
   <dimension ref="A1:AU56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AK2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="X2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E7" sqref="E7"/>
       <selection pane="topRight" activeCell="E7" sqref="E7"/>
       <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
-      <selection pane="bottomRight" activeCell="AR20" sqref="AR20"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5730,11 +5730,11 @@
         <v>414</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>1004</v>
+        <v>999</v>
       </c>
       <c r="F2" s="44"/>
       <c r="G2" s="44" t="s">
-        <v>1005</v>
+        <v>1000</v>
       </c>
       <c r="H2" s="44" t="s">
         <v>231</v>
@@ -5755,7 +5755,7 @@
         <v>430</v>
       </c>
       <c r="N2" s="44" t="s">
-        <v>1006</v>
+        <v>1001</v>
       </c>
       <c r="O2" s="44"/>
       <c r="P2" s="44" t="s">
@@ -5795,7 +5795,7 @@
         <v>578</v>
       </c>
       <c r="AJ2" s="44" t="s">
-        <v>1007</v>
+        <v>1027</v>
       </c>
       <c r="AK2" s="47" t="s">
         <v>232</v>
@@ -5840,11 +5840,11 @@
         <v>414</v>
       </c>
       <c r="E3" s="44" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="F3" s="44"/>
       <c r="G3" s="44" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="H3" s="44" t="s">
         <v>233</v>
@@ -5905,7 +5905,7 @@
         <v>579</v>
       </c>
       <c r="AJ3" s="44" t="s">
-        <v>896</v>
+        <v>1028</v>
       </c>
       <c r="AK3" s="47" t="s">
         <v>234</v>
@@ -5950,11 +5950,11 @@
         <v>140</v>
       </c>
       <c r="E4" s="44" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="F4" s="44"/>
       <c r="G4" s="44" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="H4" s="44" t="s">
         <v>421</v>
@@ -6029,7 +6029,7 @@
         <v>580</v>
       </c>
       <c r="AJ4" s="44" t="s">
-        <v>1008</v>
+        <v>1002</v>
       </c>
       <c r="AK4" s="47" t="s">
         <v>235</v>
@@ -6074,11 +6074,11 @@
         <v>140</v>
       </c>
       <c r="E5" s="44" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="F5" s="44"/>
       <c r="G5" s="44" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="H5" s="44" t="s">
         <v>422</v>
@@ -6153,7 +6153,7 @@
         <v>581</v>
       </c>
       <c r="AJ5" s="44" t="s">
-        <v>1009</v>
+        <v>1003</v>
       </c>
       <c r="AK5" s="47" t="s">
         <v>236</v>
@@ -6198,11 +6198,11 @@
         <v>140</v>
       </c>
       <c r="E6" s="44" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="F6" s="44"/>
       <c r="G6" s="44" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="H6" s="44" t="s">
         <v>423</v>
@@ -6277,7 +6277,7 @@
         <v>582</v>
       </c>
       <c r="AJ6" s="44" t="s">
-        <v>1010</v>
+        <v>1004</v>
       </c>
       <c r="AK6" s="47" t="s">
         <v>266</v>
@@ -6322,11 +6322,11 @@
         <v>140</v>
       </c>
       <c r="E7" s="44" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="F7" s="44"/>
       <c r="G7" s="44" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="H7" s="44" t="s">
         <v>419</v>
@@ -6401,7 +6401,7 @@
         <v>583</v>
       </c>
       <c r="AJ7" s="44" t="s">
-        <v>1011</v>
+        <v>1005</v>
       </c>
       <c r="AK7" s="47" t="s">
         <v>573</v>
@@ -6446,11 +6446,11 @@
         <v>140</v>
       </c>
       <c r="E8" s="44" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="F8" s="44"/>
       <c r="G8" s="44" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="H8" s="44" t="s">
         <v>420</v>
@@ -6525,7 +6525,7 @@
         <v>584</v>
       </c>
       <c r="AJ8" s="44" t="s">
-        <v>1012</v>
+        <v>1006</v>
       </c>
       <c r="AK8" s="47" t="s">
         <v>237</v>
@@ -6570,11 +6570,11 @@
         <v>414</v>
       </c>
       <c r="E9" s="44" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="F9" s="44"/>
       <c r="G9" s="44" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="H9" s="44" t="s">
         <v>238</v>
@@ -6635,7 +6635,7 @@
         <v>585</v>
       </c>
       <c r="AJ9" s="44" t="s">
-        <v>893</v>
+        <v>1029</v>
       </c>
       <c r="AK9" s="47" t="s">
         <v>239</v>
@@ -6680,11 +6680,11 @@
         <v>414</v>
       </c>
       <c r="E10" s="44" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="F10" s="44"/>
       <c r="G10" s="44" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="H10" s="44" t="s">
         <v>240</v>
@@ -6745,7 +6745,7 @@
         <v>586</v>
       </c>
       <c r="AJ10" s="44" t="s">
-        <v>974</v>
+        <v>1030</v>
       </c>
       <c r="AK10" s="47" t="s">
         <v>241</v>
@@ -6790,11 +6790,11 @@
         <v>140</v>
       </c>
       <c r="E11" s="44" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="F11" s="44"/>
       <c r="G11" s="44" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="H11" s="44" t="s">
         <v>334</v>
@@ -6855,7 +6855,7 @@
         <v>587</v>
       </c>
       <c r="AJ11" s="44" t="s">
-        <v>975</v>
+        <v>1031</v>
       </c>
       <c r="AK11" s="47" t="s">
         <v>242</v>
@@ -6900,11 +6900,11 @@
         <v>140</v>
       </c>
       <c r="E12" s="44" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="F12" s="44"/>
       <c r="G12" s="44" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="H12" s="44" t="s">
         <v>335</v>
@@ -6965,7 +6965,7 @@
         <v>588</v>
       </c>
       <c r="AJ12" s="44" t="s">
-        <v>976</v>
+        <v>1032</v>
       </c>
       <c r="AK12" s="47" t="s">
         <v>243</v>
@@ -7010,11 +7010,11 @@
         <v>414</v>
       </c>
       <c r="E13" s="44" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="F13" s="44"/>
       <c r="G13" s="44" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="H13" s="44" t="s">
         <v>244</v>
@@ -7075,7 +7075,7 @@
         <v>589</v>
       </c>
       <c r="AJ13" s="44" t="s">
-        <v>996</v>
+        <v>991</v>
       </c>
       <c r="AK13" s="47" t="s">
         <v>246</v>
@@ -7120,11 +7120,11 @@
         <v>414</v>
       </c>
       <c r="E14" s="44" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="F14" s="44"/>
       <c r="G14" s="44" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="H14" s="44" t="s">
         <v>245</v>
@@ -7185,7 +7185,7 @@
         <v>590</v>
       </c>
       <c r="AJ14" s="44" t="s">
-        <v>997</v>
+        <v>992</v>
       </c>
       <c r="AK14" s="47" t="s">
         <v>247</v>
@@ -7230,11 +7230,11 @@
         <v>414</v>
       </c>
       <c r="E15" s="44" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="F15" s="44"/>
       <c r="G15" s="44" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="H15" s="44" t="s">
         <v>248</v>
@@ -7295,7 +7295,7 @@
         <v>591</v>
       </c>
       <c r="AJ15" s="44" t="s">
-        <v>998</v>
+        <v>993</v>
       </c>
       <c r="AK15" s="47" t="s">
         <v>249</v>
@@ -7340,11 +7340,11 @@
         <v>225</v>
       </c>
       <c r="E16" s="44" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="F16" s="44"/>
       <c r="G16" s="44" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="H16" s="44" t="s">
         <v>183</v>
@@ -7419,7 +7419,7 @@
         <v>592</v>
       </c>
       <c r="AJ16" s="44" t="s">
-        <v>1013</v>
+        <v>1007</v>
       </c>
       <c r="AK16" s="44" t="s">
         <v>574</v>
@@ -7464,11 +7464,11 @@
         <v>225</v>
       </c>
       <c r="E17" s="44" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="F17" s="44"/>
       <c r="G17" s="44" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="H17" s="44" t="s">
         <v>184</v>
@@ -7543,7 +7543,7 @@
         <v>593</v>
       </c>
       <c r="AJ17" s="44" t="s">
-        <v>1014</v>
+        <v>1008</v>
       </c>
       <c r="AK17" s="44" t="s">
         <v>575</v>
@@ -7592,7 +7592,7 @@
       </c>
       <c r="F18" s="44"/>
       <c r="G18" s="44" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="H18" s="44" t="s">
         <v>185</v>
@@ -7667,7 +7667,7 @@
         <v>594</v>
       </c>
       <c r="AJ18" s="44" t="s">
-        <v>1015</v>
+        <v>1009</v>
       </c>
       <c r="AK18" s="47" t="s">
         <v>173</v>
@@ -7712,11 +7712,11 @@
         <v>225</v>
       </c>
       <c r="E19" s="44" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="F19" s="44"/>
       <c r="G19" s="44" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="H19" s="44" t="s">
         <v>185</v>
@@ -7791,7 +7791,7 @@
         <v>595</v>
       </c>
       <c r="AJ19" s="44" t="s">
-        <v>1016</v>
+        <v>1010</v>
       </c>
       <c r="AK19" s="47" t="s">
         <v>251</v>
@@ -7836,11 +7836,11 @@
         <v>225</v>
       </c>
       <c r="E20" s="44" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="F20" s="44"/>
       <c r="G20" s="44" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="H20" s="44" t="s">
         <v>185</v>
@@ -7915,7 +7915,7 @@
         <v>596</v>
       </c>
       <c r="AJ20" s="44" t="s">
-        <v>1017</v>
+        <v>1011</v>
       </c>
       <c r="AK20" s="47" t="s">
         <v>276</v>
@@ -7960,10 +7960,10 @@
         <v>225</v>
       </c>
       <c r="E21" s="44" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="G21" s="44" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="H21" s="44" t="s">
         <v>428</v>
@@ -8038,7 +8038,7 @@
         <v>597</v>
       </c>
       <c r="AJ21" s="44" t="s">
-        <v>1018</v>
+        <v>1012</v>
       </c>
       <c r="AK21" s="44" t="s">
         <v>576</v>
@@ -8083,11 +8083,11 @@
         <v>225</v>
       </c>
       <c r="E22" s="44" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="F22" s="44"/>
       <c r="G22" s="44" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="H22" s="44" t="s">
         <v>253</v>
@@ -8145,7 +8145,7 @@
         <v>598</v>
       </c>
       <c r="AJ22" s="44" t="s">
-        <v>977</v>
+        <v>972</v>
       </c>
       <c r="AK22" s="47" t="s">
         <v>254</v>
@@ -8190,11 +8190,11 @@
         <v>225</v>
       </c>
       <c r="E23" s="44" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="F23" s="44"/>
       <c r="G23" s="44" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="H23" s="44" t="s">
         <v>255</v>
@@ -8252,7 +8252,7 @@
         <v>599</v>
       </c>
       <c r="AJ23" s="44" t="s">
-        <v>978</v>
+        <v>973</v>
       </c>
       <c r="AK23" s="47" t="s">
         <v>261</v>
@@ -8297,11 +8297,11 @@
         <v>215</v>
       </c>
       <c r="E24" s="44" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="F24" s="44"/>
       <c r="G24" s="44" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="H24" s="44" t="s">
         <v>268</v>
@@ -8359,7 +8359,7 @@
         <v>600</v>
       </c>
       <c r="AJ24" s="44" t="s">
-        <v>979</v>
+        <v>974</v>
       </c>
       <c r="AK24" s="47" t="s">
         <v>277</v>
@@ -8404,11 +8404,11 @@
         <v>215</v>
       </c>
       <c r="E25" s="44" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="F25" s="44"/>
       <c r="G25" s="44" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="H25" s="44" t="s">
         <v>269</v>
@@ -8466,7 +8466,7 @@
         <v>601</v>
       </c>
       <c r="AJ25" s="44" t="s">
-        <v>980</v>
+        <v>975</v>
       </c>
       <c r="AK25" s="47" t="s">
         <v>278</v>
@@ -8511,11 +8511,11 @@
         <v>226</v>
       </c>
       <c r="E26" s="44" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="44" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>257</v>
@@ -8590,7 +8590,7 @@
         <v>602</v>
       </c>
       <c r="AJ26" s="44" t="s">
-        <v>1019</v>
+        <v>1013</v>
       </c>
       <c r="AK26" s="47" t="s">
         <v>279</v>
@@ -8635,11 +8635,11 @@
         <v>226</v>
       </c>
       <c r="E27" s="44" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="F27" s="44"/>
       <c r="G27" s="44" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="H27" s="44" t="s">
         <v>256</v>
@@ -8714,7 +8714,7 @@
         <v>603</v>
       </c>
       <c r="AJ27" s="44" t="s">
-        <v>1020</v>
+        <v>1014</v>
       </c>
       <c r="AK27" s="47" t="s">
         <v>280</v>
@@ -8759,11 +8759,11 @@
         <v>226</v>
       </c>
       <c r="E28" s="44" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="F28" s="44"/>
       <c r="G28" s="44" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="H28" s="44" t="s">
         <v>258</v>
@@ -8838,7 +8838,7 @@
         <v>604</v>
       </c>
       <c r="AJ28" s="44" t="s">
-        <v>1021</v>
+        <v>1015</v>
       </c>
       <c r="AK28" s="47" t="s">
         <v>281</v>
@@ -8883,11 +8883,11 @@
         <v>226</v>
       </c>
       <c r="E29" s="44" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="F29" s="44"/>
       <c r="G29" s="44" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="H29" s="44" t="s">
         <v>259</v>
@@ -8962,7 +8962,7 @@
         <v>605</v>
       </c>
       <c r="AJ29" s="44" t="s">
-        <v>1022</v>
+        <v>1016</v>
       </c>
       <c r="AK29" s="47" t="s">
         <v>282</v>
@@ -9007,11 +9007,11 @@
         <v>226</v>
       </c>
       <c r="E30" s="44" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="F30" s="44"/>
       <c r="G30" s="44" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="H30" s="44" t="s">
         <v>260</v>
@@ -9086,7 +9086,7 @@
         <v>606</v>
       </c>
       <c r="AJ30" s="44" t="s">
-        <v>1023</v>
+        <v>1017</v>
       </c>
       <c r="AK30" s="47" t="s">
         <v>275</v>
@@ -9135,7 +9135,7 @@
       </c>
       <c r="F31" s="44"/>
       <c r="G31" s="44" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="H31" s="44" t="s">
         <v>270</v>
@@ -9193,7 +9193,7 @@
         <v>607</v>
       </c>
       <c r="AJ31" s="44" t="s">
-        <v>981</v>
+        <v>976</v>
       </c>
       <c r="AK31" s="47" t="s">
         <v>274</v>
@@ -9242,7 +9242,7 @@
       </c>
       <c r="F32" s="44"/>
       <c r="G32" s="44" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="H32" s="44" t="s">
         <v>426</v>
@@ -9317,7 +9317,7 @@
         <v>608</v>
       </c>
       <c r="AJ32" s="44" t="s">
-        <v>1024</v>
+        <v>1018</v>
       </c>
       <c r="AK32" s="47" t="s">
         <v>267</v>
@@ -9366,7 +9366,7 @@
       </c>
       <c r="F33" s="44"/>
       <c r="G33" s="44" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="H33" s="44" t="s">
         <v>427</v>
@@ -9441,7 +9441,7 @@
         <v>609</v>
       </c>
       <c r="AJ33" s="44" t="s">
-        <v>1025</v>
+        <v>1019</v>
       </c>
       <c r="AK33" s="47" t="s">
         <v>272</v>
@@ -9489,7 +9489,7 @@
         <v>416</v>
       </c>
       <c r="G34" s="44" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="H34" s="44" t="s">
         <v>429</v>
@@ -9564,7 +9564,7 @@
         <v>610</v>
       </c>
       <c r="AJ34" s="44" t="s">
-        <v>1026</v>
+        <v>1020</v>
       </c>
       <c r="AK34" s="58" t="s">
         <v>273</v>
@@ -9613,7 +9613,7 @@
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="44" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>257</v>
@@ -9688,7 +9688,7 @@
         <v>611</v>
       </c>
       <c r="AJ35" s="44" t="s">
-        <v>1027</v>
+        <v>1021</v>
       </c>
       <c r="AK35" s="47" t="s">
         <v>283</v>
@@ -9737,7 +9737,7 @@
       </c>
       <c r="F36" s="44"/>
       <c r="G36" s="44" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="H36" s="44" t="s">
         <v>256</v>
@@ -9812,7 +9812,7 @@
         <v>612</v>
       </c>
       <c r="AJ36" s="44" t="s">
-        <v>1028</v>
+        <v>1022</v>
       </c>
       <c r="AK36" s="47" t="s">
         <v>284</v>
@@ -9861,7 +9861,7 @@
       </c>
       <c r="F37" s="44"/>
       <c r="G37" s="44" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="H37" s="44" t="s">
         <v>258</v>
@@ -9936,7 +9936,7 @@
         <v>613</v>
       </c>
       <c r="AJ37" s="44" t="s">
-        <v>1029</v>
+        <v>1023</v>
       </c>
       <c r="AK37" s="47" t="s">
         <v>285</v>
@@ -9985,7 +9985,7 @@
       </c>
       <c r="F38" s="44"/>
       <c r="G38" s="44" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="H38" s="44" t="s">
         <v>259</v>
@@ -10060,7 +10060,7 @@
         <v>614</v>
       </c>
       <c r="AJ38" s="44" t="s">
-        <v>1030</v>
+        <v>1024</v>
       </c>
       <c r="AK38" s="47" t="s">
         <v>286</v>
@@ -10109,7 +10109,7 @@
       </c>
       <c r="F39" s="44"/>
       <c r="G39" s="44" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="H39" s="44" t="s">
         <v>260</v>
@@ -10184,7 +10184,7 @@
         <v>615</v>
       </c>
       <c r="AJ39" s="44" t="s">
-        <v>1031</v>
+        <v>1025</v>
       </c>
       <c r="AK39" s="47" t="s">
         <v>287</v>
@@ -10233,7 +10233,7 @@
       </c>
       <c r="F40" s="44"/>
       <c r="G40" s="44" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="H40" s="44" t="s">
         <v>230</v>
@@ -10308,7 +10308,7 @@
         <v>616</v>
       </c>
       <c r="AJ40" s="44" t="s">
-        <v>1032</v>
+        <v>1026</v>
       </c>
       <c r="AK40" s="44" t="s">
         <v>288</v>
@@ -10357,7 +10357,7 @@
       </c>
       <c r="F41" s="44"/>
       <c r="G41" s="44" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="H41" s="44" t="s">
         <v>165</v>
@@ -10420,7 +10420,7 @@
         <v>617</v>
       </c>
       <c r="AJ41" s="44" t="s">
-        <v>982</v>
+        <v>977</v>
       </c>
       <c r="AK41" s="44" t="s">
         <v>577</v>
@@ -10469,7 +10469,7 @@
       </c>
       <c r="F42" s="44"/>
       <c r="G42" s="44" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="H42" s="44" t="s">
         <v>296</v>
@@ -10530,7 +10530,7 @@
         <v>618</v>
       </c>
       <c r="AJ42" s="44" t="s">
-        <v>988</v>
+        <v>983</v>
       </c>
       <c r="AK42" s="44" t="s">
         <v>291</v>
@@ -10579,7 +10579,7 @@
       </c>
       <c r="F43" s="44"/>
       <c r="G43" s="44" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="H43" s="44" t="s">
         <v>297</v>
@@ -10640,7 +10640,7 @@
         <v>619</v>
       </c>
       <c r="AJ43" s="44" t="s">
-        <v>989</v>
+        <v>984</v>
       </c>
       <c r="AK43" s="44" t="s">
         <v>292</v>
@@ -10689,7 +10689,7 @@
       </c>
       <c r="F44" s="47"/>
       <c r="G44" s="44" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="H44" s="44" t="s">
         <v>295</v>
@@ -10750,7 +10750,7 @@
         <v>620</v>
       </c>
       <c r="AJ44" s="44" t="s">
-        <v>990</v>
+        <v>985</v>
       </c>
       <c r="AK44" s="47" t="s">
         <v>293</v>
@@ -10799,7 +10799,7 @@
       </c>
       <c r="F45" s="47"/>
       <c r="G45" s="44" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="H45" s="44" t="s">
         <v>298</v>
@@ -10860,7 +10860,7 @@
         <v>621</v>
       </c>
       <c r="AJ45" s="44" t="s">
-        <v>991</v>
+        <v>986</v>
       </c>
       <c r="AK45" s="47" t="s">
         <v>294</v>
@@ -10909,7 +10909,7 @@
       </c>
       <c r="F46" s="44"/>
       <c r="G46" s="44" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="H46" s="44" t="s">
         <v>166</v>
@@ -10970,7 +10970,7 @@
         <v>622</v>
       </c>
       <c r="AJ46" s="44" t="s">
-        <v>992</v>
+        <v>987</v>
       </c>
       <c r="AK46" s="47" t="s">
         <v>174</v>
@@ -11019,7 +11019,7 @@
       </c>
       <c r="F47" s="44"/>
       <c r="G47" s="44" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="H47" s="44" t="s">
         <v>186</v>
@@ -11080,7 +11080,7 @@
         <v>623</v>
       </c>
       <c r="AJ47" s="44" t="s">
-        <v>993</v>
+        <v>988</v>
       </c>
       <c r="AK47" s="44" t="s">
         <v>175</v>
@@ -11129,7 +11129,7 @@
       </c>
       <c r="F48" s="44"/>
       <c r="G48" s="44" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="H48" s="44" t="s">
         <v>187</v>
@@ -11192,7 +11192,7 @@
         <v>624</v>
       </c>
       <c r="AJ48" s="44" t="s">
-        <v>983</v>
+        <v>978</v>
       </c>
       <c r="AK48" s="44" t="s">
         <v>176</v>
@@ -11241,7 +11241,7 @@
       </c>
       <c r="F49" s="44"/>
       <c r="G49" s="44" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="H49" s="44" t="s">
         <v>169</v>
@@ -11304,7 +11304,7 @@
         <v>625</v>
       </c>
       <c r="AJ49" s="44" t="s">
-        <v>984</v>
+        <v>979</v>
       </c>
       <c r="AK49" s="47" t="s">
         <v>177</v>
@@ -11353,7 +11353,7 @@
       </c>
       <c r="F50" s="44"/>
       <c r="G50" s="44" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="H50" s="44" t="s">
         <v>170</v>
@@ -11416,7 +11416,7 @@
         <v>626</v>
       </c>
       <c r="AJ50" s="44" t="s">
-        <v>985</v>
+        <v>980</v>
       </c>
       <c r="AK50" s="47" t="s">
         <v>178</v>
@@ -11465,7 +11465,7 @@
       </c>
       <c r="F51" s="44"/>
       <c r="G51" s="44" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="H51" s="44" t="s">
         <v>171</v>
@@ -11528,7 +11528,7 @@
         <v>627</v>
       </c>
       <c r="AJ51" s="44" t="s">
-        <v>986</v>
+        <v>981</v>
       </c>
       <c r="AK51" s="47" t="s">
         <v>179</v>
@@ -11577,7 +11577,7 @@
       </c>
       <c r="F52" s="44"/>
       <c r="G52" s="44" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="H52" s="44" t="s">
         <v>172</v>
@@ -11640,7 +11640,7 @@
         <v>628</v>
       </c>
       <c r="AJ52" s="44" t="s">
-        <v>987</v>
+        <v>982</v>
       </c>
       <c r="AK52" s="47" t="s">
         <v>180</v>
@@ -11680,7 +11680,7 @@
         <v>863</v>
       </c>
       <c r="C53" s="44" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="D53" s="44" t="s">
         <v>140</v>
@@ -11690,7 +11690,7 @@
       </c>
       <c r="F53" s="44"/>
       <c r="G53" s="44" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="H53" s="44" t="s">
         <v>852</v>
@@ -11771,7 +11771,7 @@
         <v>883</v>
       </c>
       <c r="AJ53" s="44" t="s">
-        <v>994</v>
+        <v>989</v>
       </c>
       <c r="AK53" s="44" t="s">
         <v>867</v>
@@ -11821,7 +11821,7 @@
       </c>
       <c r="F54" s="44"/>
       <c r="G54" s="44" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="H54" s="44" t="s">
         <v>855</v>
@@ -11886,7 +11886,7 @@
         <v>884</v>
       </c>
       <c r="AJ54" s="44" t="s">
-        <v>995</v>
+        <v>990</v>
       </c>
       <c r="AK54" s="44" t="s">
         <v>856</v>
@@ -11936,7 +11936,7 @@
       </c>
       <c r="F55" s="44"/>
       <c r="G55" s="44" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="H55" s="44" t="s">
         <v>857</v>
@@ -12004,7 +12004,7 @@
         <v>889</v>
       </c>
       <c r="AK55" s="44" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="AL55" s="44" t="s">
         <v>188</v>
@@ -12051,7 +12051,7 @@
       </c>
       <c r="F56" s="44"/>
       <c r="G56" s="44" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="H56" s="44" t="s">
         <v>860</v>
@@ -12732,7 +12732,7 @@
         <v>562</v>
       </c>
       <c r="F3" t="s">
-        <v>999</v>
+        <v>994</v>
       </c>
       <c r="G3" t="s">
         <v>558</v>
@@ -12755,7 +12755,7 @@
         <v>561</v>
       </c>
       <c r="F4" t="s">
-        <v>1000</v>
+        <v>995</v>
       </c>
       <c r="G4" t="s">
         <v>558</v>
@@ -12778,7 +12778,7 @@
         <v>563</v>
       </c>
       <c r="F5" t="s">
-        <v>1001</v>
+        <v>996</v>
       </c>
       <c r="G5" t="s">
         <v>558</v>
@@ -12801,7 +12801,7 @@
         <v>564</v>
       </c>
       <c r="F6" t="s">
-        <v>1002</v>
+        <v>997</v>
       </c>
       <c r="G6" t="s">
         <v>558</v>
@@ -12824,7 +12824,7 @@
         <v>560</v>
       </c>
       <c r="F7" t="s">
-        <v>1003</v>
+        <v>998</v>
       </c>
       <c r="G7" t="s">
         <v>558</v>

</xml_diff>

<commit_message>
made variable names unique
</commit_message>
<xml_diff>
--- a/ontology_cip_2015_10_26_short.xlsx
+++ b/ontology_cip_2015_10_26_short.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2363" uniqueCount="1034">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2363" uniqueCount="1089">
   <si>
     <t>List of columns in template and short description:</t>
   </si>
@@ -3146,6 +3146,171 @@
   </si>
   <si>
     <t>Z. Huaman</t>
+  </si>
+  <si>
+    <t>variable Number of plants planted</t>
+  </si>
+  <si>
+    <t>variable Number of plants established</t>
+  </si>
+  <si>
+    <t>variable Virus symptoms 1</t>
+  </si>
+  <si>
+    <t>variable Virus symptoms 2</t>
+  </si>
+  <si>
+    <t>variable Vine vigor 1</t>
+  </si>
+  <si>
+    <t>variable Early Blight: (Alternaria) 1</t>
+  </si>
+  <si>
+    <t>variable Early Blight: (Alternaria) 2</t>
+  </si>
+  <si>
+    <t>variable Number of plants harvested</t>
+  </si>
+  <si>
+    <t>variable Number of plants with storage roots</t>
+  </si>
+  <si>
+    <t>variable Number of commercial storage roots/plot</t>
+  </si>
+  <si>
+    <t>variable Number of non-commercial storage roots/plot</t>
+  </si>
+  <si>
+    <t>variable Weight of commercial storage roots/net plot in kg</t>
+  </si>
+  <si>
+    <t>variable Weight of non-commercial storage roots/net plot in kg</t>
+  </si>
+  <si>
+    <t>variable Weight of vines/net plot in kg</t>
+  </si>
+  <si>
+    <t>variable Predominant Skin color</t>
+  </si>
+  <si>
+    <t>variable Predominant Flesh color</t>
+  </si>
+  <si>
+    <t>variable Storage root size</t>
+  </si>
+  <si>
+    <t>variable Storage root form</t>
+  </si>
+  <si>
+    <t>variable Storage root damages</t>
+  </si>
+  <si>
+    <t>variable Reaction to sweet potato weevil 1</t>
+  </si>
+  <si>
+    <t>variable Fresh weight of storage root samples</t>
+  </si>
+  <si>
+    <t>variable Dry weight of storage root samples</t>
+  </si>
+  <si>
+    <t>variable Fresh weight of vines</t>
+  </si>
+  <si>
+    <t>variable Dry weight of vines</t>
+  </si>
+  <si>
+    <t>variable Fibers in cooked samples 1</t>
+  </si>
+  <si>
+    <t>variable Storage root sweetness 1</t>
+  </si>
+  <si>
+    <t>variable Storage root texture 1</t>
+  </si>
+  <si>
+    <t>variable Overall taste of cooked sample 1</t>
+  </si>
+  <si>
+    <t>variable Overall appearance of cooked sample 1</t>
+  </si>
+  <si>
+    <t>variable Plot size at harvest</t>
+  </si>
+  <si>
+    <t>variable Vine vigor 2</t>
+  </si>
+  <si>
+    <t>variable Virus symptoms 3</t>
+  </si>
+  <si>
+    <t>variable Reaction to sweet potato weevil 2</t>
+  </si>
+  <si>
+    <t>variable Fibers in cooked samples 2</t>
+  </si>
+  <si>
+    <t>variable Storage root sweetness 2</t>
+  </si>
+  <si>
+    <t>variable Storage root texture 2</t>
+  </si>
+  <si>
+    <t>variable Overall taste of cooked sample 2</t>
+  </si>
+  <si>
+    <t>variable Overall appearance of cooked sample 2</t>
+  </si>
+  <si>
+    <t>variable Sprouting ability</t>
+  </si>
+  <si>
+    <t>variable Protein content</t>
+  </si>
+  <si>
+    <t>variable Content of iron on dry weight basis</t>
+  </si>
+  <si>
+    <t>variable Content of zinc on dry weight basis</t>
+  </si>
+  <si>
+    <t>variable Content of calcium on dry weight basis</t>
+  </si>
+  <si>
+    <t>variable Content of magnesium on dry weight basis</t>
+  </si>
+  <si>
+    <t>variable Beta carotene content</t>
+  </si>
+  <si>
+    <t>variable Total carotenoids</t>
+  </si>
+  <si>
+    <t>variable Storage root starch content</t>
+  </si>
+  <si>
+    <t>variable Fructose content</t>
+  </si>
+  <si>
+    <t>variable Glucose content</t>
+  </si>
+  <si>
+    <t>variable Sucrose content</t>
+  </si>
+  <si>
+    <t>variable Maltose content</t>
+  </si>
+  <si>
+    <t>variable Yield of total roots per hectar</t>
+  </si>
+  <si>
+    <t>variable Storage root dry matter content</t>
+  </si>
+  <si>
+    <t>variable Survival index</t>
+  </si>
+  <si>
+    <t>variable Harvest index</t>
   </si>
 </sst>
 </file>
@@ -5521,11 +5686,11 @@
   <dimension ref="A1:AV56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AM2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AG2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E7" sqref="E7"/>
       <selection pane="topRight" activeCell="E7" sqref="E7"/>
       <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
-      <selection pane="bottomRight" activeCell="AR16" sqref="AR16"/>
+      <selection pane="bottomRight" activeCell="AJ8" sqref="AJ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5802,7 +5967,7 @@
         <v>576</v>
       </c>
       <c r="AJ2" s="44" t="s">
-        <v>231</v>
+        <v>1034</v>
       </c>
       <c r="AK2" s="44" t="s">
         <v>1026</v>
@@ -5915,7 +6080,7 @@
         <v>577</v>
       </c>
       <c r="AJ3" s="44" t="s">
-        <v>233</v>
+        <v>1035</v>
       </c>
       <c r="AK3" s="44" t="s">
         <v>1027</v>
@@ -6042,7 +6207,7 @@
         <v>578</v>
       </c>
       <c r="AJ4" s="44" t="s">
-        <v>265</v>
+        <v>1036</v>
       </c>
       <c r="AK4" s="44" t="s">
         <v>1000</v>
@@ -6169,7 +6334,7 @@
         <v>579</v>
       </c>
       <c r="AJ5" s="44" t="s">
-        <v>264</v>
+        <v>1037</v>
       </c>
       <c r="AK5" s="44" t="s">
         <v>1001</v>
@@ -6296,7 +6461,7 @@
         <v>580</v>
       </c>
       <c r="AJ6" s="44" t="s">
-        <v>374</v>
+        <v>1038</v>
       </c>
       <c r="AK6" s="44" t="s">
         <v>1002</v>
@@ -6423,7 +6588,7 @@
         <v>581</v>
       </c>
       <c r="AJ7" s="44" t="s">
-        <v>263</v>
+        <v>1039</v>
       </c>
       <c r="AK7" s="44" t="s">
         <v>1003</v>
@@ -6550,7 +6715,7 @@
         <v>582</v>
       </c>
       <c r="AJ8" s="44" t="s">
-        <v>262</v>
+        <v>1040</v>
       </c>
       <c r="AK8" s="44" t="s">
         <v>1004</v>
@@ -6663,7 +6828,7 @@
         <v>583</v>
       </c>
       <c r="AJ9" s="44" t="s">
-        <v>238</v>
+        <v>1041</v>
       </c>
       <c r="AK9" s="44" t="s">
         <v>1028</v>
@@ -6776,7 +6941,7 @@
         <v>584</v>
       </c>
       <c r="AJ10" s="44" t="s">
-        <v>240</v>
+        <v>1042</v>
       </c>
       <c r="AK10" s="44" t="s">
         <v>1029</v>
@@ -6889,7 +7054,7 @@
         <v>585</v>
       </c>
       <c r="AJ11" s="44" t="s">
-        <v>332</v>
+        <v>1043</v>
       </c>
       <c r="AK11" s="44" t="s">
         <v>1030</v>
@@ -7002,7 +7167,7 @@
         <v>586</v>
       </c>
       <c r="AJ12" s="44" t="s">
-        <v>333</v>
+        <v>1044</v>
       </c>
       <c r="AK12" s="44" t="s">
         <v>1031</v>
@@ -7115,7 +7280,7 @@
         <v>587</v>
       </c>
       <c r="AJ13" s="44" t="s">
-        <v>244</v>
+        <v>1045</v>
       </c>
       <c r="AK13" s="44" t="s">
         <v>989</v>
@@ -7228,7 +7393,7 @@
         <v>588</v>
       </c>
       <c r="AJ14" s="44" t="s">
-        <v>245</v>
+        <v>1046</v>
       </c>
       <c r="AK14" s="44" t="s">
         <v>990</v>
@@ -7341,7 +7506,7 @@
         <v>589</v>
       </c>
       <c r="AJ15" s="44" t="s">
-        <v>248</v>
+        <v>1047</v>
       </c>
       <c r="AK15" s="44" t="s">
         <v>991</v>
@@ -7468,7 +7633,7 @@
         <v>590</v>
       </c>
       <c r="AJ16" s="44" t="s">
-        <v>162</v>
+        <v>1048</v>
       </c>
       <c r="AK16" s="44" t="s">
         <v>1005</v>
@@ -7595,7 +7760,7 @@
         <v>591</v>
       </c>
       <c r="AJ17" s="44" t="s">
-        <v>163</v>
+        <v>1049</v>
       </c>
       <c r="AK17" s="44" t="s">
         <v>1006</v>
@@ -7722,7 +7887,7 @@
         <v>592</v>
       </c>
       <c r="AJ18" s="44" t="s">
-        <v>164</v>
+        <v>1050</v>
       </c>
       <c r="AK18" s="44" t="s">
         <v>1007</v>
@@ -7849,7 +8014,7 @@
         <v>593</v>
       </c>
       <c r="AJ19" s="44" t="s">
-        <v>250</v>
+        <v>1051</v>
       </c>
       <c r="AK19" s="44" t="s">
         <v>1008</v>
@@ -7976,7 +8141,7 @@
         <v>594</v>
       </c>
       <c r="AJ20" s="44" t="s">
-        <v>252</v>
+        <v>1052</v>
       </c>
       <c r="AK20" s="44" t="s">
         <v>1009</v>
@@ -8102,7 +8267,7 @@
         <v>595</v>
       </c>
       <c r="AJ21" s="40" t="s">
-        <v>289</v>
+        <v>1053</v>
       </c>
       <c r="AK21" s="44" t="s">
         <v>1010</v>
@@ -8212,7 +8377,7 @@
         <v>596</v>
       </c>
       <c r="AJ22" s="44" t="s">
-        <v>253</v>
+        <v>1054</v>
       </c>
       <c r="AK22" s="44" t="s">
         <v>970</v>
@@ -8322,7 +8487,7 @@
         <v>597</v>
       </c>
       <c r="AJ23" s="44" t="s">
-        <v>255</v>
+        <v>1055</v>
       </c>
       <c r="AK23" s="44" t="s">
         <v>971</v>
@@ -8432,7 +8597,7 @@
         <v>598</v>
       </c>
       <c r="AJ24" s="44" t="s">
-        <v>268</v>
+        <v>1056</v>
       </c>
       <c r="AK24" s="44" t="s">
         <v>972</v>
@@ -8542,7 +8707,7 @@
         <v>599</v>
       </c>
       <c r="AJ25" s="44" t="s">
-        <v>269</v>
+        <v>1057</v>
       </c>
       <c r="AK25" s="44" t="s">
         <v>973</v>
@@ -8669,7 +8834,7 @@
         <v>600</v>
       </c>
       <c r="AJ26" s="3" t="s">
-        <v>835</v>
+        <v>1058</v>
       </c>
       <c r="AK26" s="44" t="s">
         <v>1011</v>
@@ -8796,7 +8961,7 @@
         <v>601</v>
       </c>
       <c r="AJ27" s="44" t="s">
-        <v>837</v>
+        <v>1059</v>
       </c>
       <c r="AK27" s="44" t="s">
         <v>1012</v>
@@ -8923,7 +9088,7 @@
         <v>602</v>
       </c>
       <c r="AJ28" s="44" t="s">
-        <v>838</v>
+        <v>1060</v>
       </c>
       <c r="AK28" s="44" t="s">
         <v>1013</v>
@@ -9050,7 +9215,7 @@
         <v>603</v>
       </c>
       <c r="AJ29" s="44" t="s">
-        <v>839</v>
+        <v>1061</v>
       </c>
       <c r="AK29" s="44" t="s">
         <v>1014</v>
@@ -9177,7 +9342,7 @@
         <v>604</v>
       </c>
       <c r="AJ30" s="44" t="s">
-        <v>840</v>
+        <v>1062</v>
       </c>
       <c r="AK30" s="44" t="s">
         <v>1015</v>
@@ -9287,7 +9452,7 @@
         <v>605</v>
       </c>
       <c r="AJ31" s="44" t="s">
-        <v>270</v>
+        <v>1063</v>
       </c>
       <c r="AK31" s="44" t="s">
         <v>974</v>
@@ -9414,7 +9579,7 @@
         <v>606</v>
       </c>
       <c r="AJ32" s="44" t="s">
-        <v>375</v>
+        <v>1064</v>
       </c>
       <c r="AK32" s="44" t="s">
         <v>1016</v>
@@ -9541,7 +9706,7 @@
         <v>607</v>
       </c>
       <c r="AJ33" s="44" t="s">
-        <v>271</v>
+        <v>1065</v>
       </c>
       <c r="AK33" s="44" t="s">
         <v>1017</v>
@@ -9667,7 +9832,7 @@
         <v>608</v>
       </c>
       <c r="AJ34" s="40" t="s">
-        <v>290</v>
+        <v>1066</v>
       </c>
       <c r="AK34" s="44" t="s">
         <v>1018</v>
@@ -9794,7 +9959,7 @@
         <v>609</v>
       </c>
       <c r="AJ35" s="3" t="s">
-        <v>836</v>
+        <v>1067</v>
       </c>
       <c r="AK35" s="44" t="s">
         <v>1019</v>
@@ -9921,7 +10086,7 @@
         <v>610</v>
       </c>
       <c r="AJ36" s="44" t="s">
-        <v>841</v>
+        <v>1068</v>
       </c>
       <c r="AK36" s="44" t="s">
         <v>1020</v>
@@ -10048,7 +10213,7 @@
         <v>611</v>
       </c>
       <c r="AJ37" s="44" t="s">
-        <v>842</v>
+        <v>1069</v>
       </c>
       <c r="AK37" s="44" t="s">
         <v>1021</v>
@@ -10175,7 +10340,7 @@
         <v>612</v>
       </c>
       <c r="AJ38" s="44" t="s">
-        <v>843</v>
+        <v>1070</v>
       </c>
       <c r="AK38" s="44" t="s">
         <v>1022</v>
@@ -10302,7 +10467,7 @@
         <v>613</v>
       </c>
       <c r="AJ39" s="44" t="s">
-        <v>844</v>
+        <v>1071</v>
       </c>
       <c r="AK39" s="44" t="s">
         <v>1023</v>
@@ -10429,7 +10594,7 @@
         <v>614</v>
       </c>
       <c r="AJ40" s="44" t="s">
-        <v>230</v>
+        <v>1072</v>
       </c>
       <c r="AK40" s="44" t="s">
         <v>1024</v>
@@ -10544,7 +10709,7 @@
         <v>615</v>
       </c>
       <c r="AJ41" s="44" t="s">
-        <v>165</v>
+        <v>1073</v>
       </c>
       <c r="AK41" s="44" t="s">
         <v>975</v>
@@ -10657,7 +10822,7 @@
         <v>616</v>
       </c>
       <c r="AJ42" s="44" t="s">
-        <v>296</v>
+        <v>1074</v>
       </c>
       <c r="AK42" s="44" t="s">
         <v>981</v>
@@ -10770,7 +10935,7 @@
         <v>617</v>
       </c>
       <c r="AJ43" s="44" t="s">
-        <v>297</v>
+        <v>1075</v>
       </c>
       <c r="AK43" s="44" t="s">
         <v>982</v>
@@ -10883,7 +11048,7 @@
         <v>618</v>
       </c>
       <c r="AJ44" s="44" t="s">
-        <v>295</v>
+        <v>1076</v>
       </c>
       <c r="AK44" s="44" t="s">
         <v>983</v>
@@ -10996,7 +11161,7 @@
         <v>619</v>
       </c>
       <c r="AJ45" s="44" t="s">
-        <v>298</v>
+        <v>1077</v>
       </c>
       <c r="AK45" s="44" t="s">
         <v>984</v>
@@ -11109,7 +11274,7 @@
         <v>620</v>
       </c>
       <c r="AJ46" s="44" t="s">
-        <v>166</v>
+        <v>1078</v>
       </c>
       <c r="AK46" s="44" t="s">
         <v>985</v>
@@ -11222,7 +11387,7 @@
         <v>621</v>
       </c>
       <c r="AJ47" s="44" t="s">
-        <v>167</v>
+        <v>1079</v>
       </c>
       <c r="AK47" s="44" t="s">
         <v>986</v>
@@ -11337,7 +11502,7 @@
         <v>622</v>
       </c>
       <c r="AJ48" s="44" t="s">
-        <v>168</v>
+        <v>1080</v>
       </c>
       <c r="AK48" s="44" t="s">
         <v>976</v>
@@ -11452,7 +11617,7 @@
         <v>623</v>
       </c>
       <c r="AJ49" s="44" t="s">
-        <v>169</v>
+        <v>1081</v>
       </c>
       <c r="AK49" s="44" t="s">
         <v>977</v>
@@ -11567,7 +11732,7 @@
         <v>624</v>
       </c>
       <c r="AJ50" s="44" t="s">
-        <v>170</v>
+        <v>1082</v>
       </c>
       <c r="AK50" s="44" t="s">
         <v>978</v>
@@ -11682,7 +11847,7 @@
         <v>625</v>
       </c>
       <c r="AJ51" s="44" t="s">
-        <v>171</v>
+        <v>1083</v>
       </c>
       <c r="AK51" s="44" t="s">
         <v>979</v>
@@ -11797,7 +11962,7 @@
         <v>626</v>
       </c>
       <c r="AJ52" s="44" t="s">
-        <v>172</v>
+        <v>1084</v>
       </c>
       <c r="AK52" s="44" t="s">
         <v>980</v>
@@ -11931,7 +12096,7 @@
         <v>881</v>
       </c>
       <c r="AJ53" s="44" t="s">
-        <v>892</v>
+        <v>1085</v>
       </c>
       <c r="AK53" s="44" t="s">
         <v>987</v>
@@ -12049,7 +12214,7 @@
         <v>882</v>
       </c>
       <c r="AJ54" s="44" t="s">
-        <v>853</v>
+        <v>1086</v>
       </c>
       <c r="AK54" s="44" t="s">
         <v>988</v>
@@ -12167,7 +12332,7 @@
         <v>883</v>
       </c>
       <c r="AJ55" s="44" t="s">
-        <v>855</v>
+        <v>1087</v>
       </c>
       <c r="AK55" s="44" t="s">
         <v>887</v>
@@ -12303,7 +12468,7 @@
         <v>884</v>
       </c>
       <c r="AJ56" s="44" t="s">
-        <v>856</v>
+        <v>1088</v>
       </c>
       <c r="AK56" s="44" t="s">
         <v>888</v>

</xml_diff>

<commit_message>
Added new column in spreadsheet 'Variable label'. This column is used as a 'name' equivalent for the OBO file. The 'Variable name' is used as synonym. 'Variable labels' were re-written in humand readable format and distinct from trait.
</commit_message>
<xml_diff>
--- a/ontology_cip_2015_10_26_short.xlsx
+++ b/ontology_cip_2015_10_26_short.xlsx
@@ -3142,175 +3142,175 @@
     <t>PltNCR_Ct_plplot</t>
   </si>
   <si>
-    <t>Variable IBP name</t>
-  </si>
-  <si>
     <t>Z. Huaman</t>
   </si>
   <si>
-    <t>variable Number of plants planted</t>
-  </si>
-  <si>
-    <t>variable Number of plants established</t>
-  </si>
-  <si>
-    <t>variable Virus symptoms 1</t>
-  </si>
-  <si>
-    <t>variable Virus symptoms 2</t>
-  </si>
-  <si>
-    <t>variable Vine vigor 1</t>
-  </si>
-  <si>
-    <t>variable Early Blight: (Alternaria) 1</t>
-  </si>
-  <si>
-    <t>variable Early Blight: (Alternaria) 2</t>
-  </si>
-  <si>
-    <t>variable Number of plants harvested</t>
-  </si>
-  <si>
-    <t>variable Number of plants with storage roots</t>
-  </si>
-  <si>
-    <t>variable Number of commercial storage roots/plot</t>
-  </si>
-  <si>
-    <t>variable Number of non-commercial storage roots/plot</t>
-  </si>
-  <si>
-    <t>variable Weight of commercial storage roots/net plot in kg</t>
-  </si>
-  <si>
-    <t>variable Weight of non-commercial storage roots/net plot in kg</t>
-  </si>
-  <si>
-    <t>variable Weight of vines/net plot in kg</t>
-  </si>
-  <si>
-    <t>variable Predominant Skin color</t>
-  </si>
-  <si>
-    <t>variable Predominant Flesh color</t>
-  </si>
-  <si>
-    <t>variable Storage root size</t>
-  </si>
-  <si>
-    <t>variable Storage root form</t>
-  </si>
-  <si>
-    <t>variable Storage root damages</t>
-  </si>
-  <si>
-    <t>variable Reaction to sweet potato weevil 1</t>
-  </si>
-  <si>
-    <t>variable Fresh weight of storage root samples</t>
-  </si>
-  <si>
-    <t>variable Dry weight of storage root samples</t>
-  </si>
-  <si>
-    <t>variable Fresh weight of vines</t>
-  </si>
-  <si>
-    <t>variable Dry weight of vines</t>
-  </si>
-  <si>
-    <t>variable Fibers in cooked samples 1</t>
-  </si>
-  <si>
-    <t>variable Storage root sweetness 1</t>
-  </si>
-  <si>
-    <t>variable Storage root texture 1</t>
-  </si>
-  <si>
-    <t>variable Overall taste of cooked sample 1</t>
-  </si>
-  <si>
-    <t>variable Overall appearance of cooked sample 1</t>
-  </si>
-  <si>
-    <t>variable Plot size at harvest</t>
-  </si>
-  <si>
-    <t>variable Vine vigor 2</t>
-  </si>
-  <si>
-    <t>variable Virus symptoms 3</t>
-  </si>
-  <si>
-    <t>variable Reaction to sweet potato weevil 2</t>
-  </si>
-  <si>
-    <t>variable Fibers in cooked samples 2</t>
-  </si>
-  <si>
-    <t>variable Storage root sweetness 2</t>
-  </si>
-  <si>
-    <t>variable Storage root texture 2</t>
-  </si>
-  <si>
-    <t>variable Overall taste of cooked sample 2</t>
-  </si>
-  <si>
-    <t>variable Overall appearance of cooked sample 2</t>
-  </si>
-  <si>
-    <t>variable Sprouting ability</t>
-  </si>
-  <si>
-    <t>variable Protein content</t>
-  </si>
-  <si>
-    <t>variable Content of iron on dry weight basis</t>
-  </si>
-  <si>
-    <t>variable Content of zinc on dry weight basis</t>
-  </si>
-  <si>
-    <t>variable Content of calcium on dry weight basis</t>
-  </si>
-  <si>
-    <t>variable Content of magnesium on dry weight basis</t>
-  </si>
-  <si>
-    <t>variable Beta carotene content</t>
-  </si>
-  <si>
-    <t>variable Total carotenoids</t>
-  </si>
-  <si>
-    <t>variable Storage root starch content</t>
-  </si>
-  <si>
-    <t>variable Fructose content</t>
-  </si>
-  <si>
-    <t>variable Glucose content</t>
-  </si>
-  <si>
-    <t>variable Sucrose content</t>
-  </si>
-  <si>
-    <t>variable Maltose content</t>
-  </si>
-  <si>
-    <t>variable Yield of total roots per hectar</t>
-  </si>
-  <si>
-    <t>variable Storage root dry matter content</t>
-  </si>
-  <si>
-    <t>variable Survival index</t>
-  </si>
-  <si>
-    <t>variable Harvest index</t>
+    <t>Virus symptoms 1 estimating 1-9</t>
+  </si>
+  <si>
+    <t>Virus symptoms 2 estimating 1-9</t>
+  </si>
+  <si>
+    <t>Vine vigor 1 estimating 1-9</t>
+  </si>
+  <si>
+    <t>Early Blight 2 symptoms estimating 1-9</t>
+  </si>
+  <si>
+    <t>Early Blight 1 symptoms estimating 1-9</t>
+  </si>
+  <si>
+    <t>Variable label</t>
+  </si>
+  <si>
+    <t>Predominant Skin color estimating 1-9</t>
+  </si>
+  <si>
+    <t>Predominant Flesh color estimating 1-9</t>
+  </si>
+  <si>
+    <t>Storage root size estimating 1-9</t>
+  </si>
+  <si>
+    <t>Storage root form estimating 1-9</t>
+  </si>
+  <si>
+    <t>Storage root damages estimatimg 1-9</t>
+  </si>
+  <si>
+    <t>Sweet potato weevil symptoms 1 estimating 1-9</t>
+  </si>
+  <si>
+    <t>Weight of commercial storage roots measuring kg per plot</t>
+  </si>
+  <si>
+    <t>Weight of non-commercial storage roots measuring kg per plot</t>
+  </si>
+  <si>
+    <t>Weight of vines measuring kg per plot</t>
+  </si>
+  <si>
+    <t>Dry weight of storage root samples measuring g of sample</t>
+  </si>
+  <si>
+    <t>Fresh weight of storage root samples measuring g of sample</t>
+  </si>
+  <si>
+    <t>Fresh weight of vines measuring g of sample</t>
+  </si>
+  <si>
+    <t>Dry weight of vines measuring g of sample</t>
+  </si>
+  <si>
+    <t>Fibers in cooked samples 1 estimating 1-9</t>
+  </si>
+  <si>
+    <t>Storage root sweetness 1 estimating 1-9</t>
+  </si>
+  <si>
+    <t>Storage root texture 1 estimating 1-9</t>
+  </si>
+  <si>
+    <t>Overall taste of cooked sample 1 estimating 1-9</t>
+  </si>
+  <si>
+    <t>Overall appearance of cooked sample 1 estimating 1-9</t>
+  </si>
+  <si>
+    <t>Vine vigor 2 estimating 1-9</t>
+  </si>
+  <si>
+    <t>Virus symptoms 3 estimating 1-9</t>
+  </si>
+  <si>
+    <t>Sweet potato weevil symptom 2 estimating 1-9</t>
+  </si>
+  <si>
+    <t>Fibers in cooked samples 2 estimating 1-9</t>
+  </si>
+  <si>
+    <t>Storage root sweetness 2 estimating 1-9</t>
+  </si>
+  <si>
+    <t>Storage root texture 2 estimating 1-9</t>
+  </si>
+  <si>
+    <t>Overall taste of cooked sample 2 estimating 1-9</t>
+  </si>
+  <si>
+    <t>Overall appearance of cooked sample 2 estimating 1-9</t>
+  </si>
+  <si>
+    <t>Sprouting ability estimating 1-9</t>
+  </si>
+  <si>
+    <t>Protein content measuring percent</t>
+  </si>
+  <si>
+    <t>Content of iron on dry weight basis measuring mg per 100g</t>
+  </si>
+  <si>
+    <t>Content of zinc on dry weight basis measuring mg per 100g</t>
+  </si>
+  <si>
+    <t>Content of calcium on dry weight basis measuringm g per 100g</t>
+  </si>
+  <si>
+    <t>Content of magnesium on dry weight basis measuring mg per 100g</t>
+  </si>
+  <si>
+    <t>Beta carotene content measuring mg per 100g</t>
+  </si>
+  <si>
+    <t>Total carotenoids measuring mg per 100g</t>
+  </si>
+  <si>
+    <t>Storage root starch content measuring percent</t>
+  </si>
+  <si>
+    <t>Fructose content measuring percent</t>
+  </si>
+  <si>
+    <t>Glucose content measuring percent</t>
+  </si>
+  <si>
+    <t>Sucrose content measuring percent</t>
+  </si>
+  <si>
+    <t>Maltose content measuring percent</t>
+  </si>
+  <si>
+    <t>Yield of total roots per hectar computing tons per ha</t>
+  </si>
+  <si>
+    <t>Storage root dry matter content computing percent</t>
+  </si>
+  <si>
+    <t>Survival index computing percent</t>
+  </si>
+  <si>
+    <t>Harvest index computing percent</t>
+  </si>
+  <si>
+    <t>Plot size at harvest measuring square meter of net plot</t>
+  </si>
+  <si>
+    <t>Plants planted counting number per plot</t>
+  </si>
+  <si>
+    <t>Plants established counting number per plot</t>
+  </si>
+  <si>
+    <t>Plants harvested counting number per plot</t>
+  </si>
+  <si>
+    <t>Plants with storage roots counting number per plot</t>
+  </si>
+  <si>
+    <t>Number of commercial storage roots counting number per plot</t>
+  </si>
+  <si>
+    <t>Number of non-commercial storage roots counting number per plot</t>
   </si>
 </sst>
 </file>
@@ -5686,18 +5686,18 @@
   <dimension ref="A1:AV56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AG2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AJ2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E7" sqref="E7"/>
       <selection pane="topRight" activeCell="E7" sqref="E7"/>
       <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
-      <selection pane="bottomRight" activeCell="AJ8" sqref="AJ8"/>
+      <selection pane="bottomRight" activeCell="AJ13" sqref="AJ13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" style="3" customWidth="1"/>
     <col min="2" max="2" width="18" style="40" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" style="40" customWidth="1"/>
+    <col min="3" max="3" width="49.7109375" style="40" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" style="40" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" style="40" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" style="40" customWidth="1"/>
@@ -5713,7 +5713,7 @@
     <col min="16" max="16" width="25" style="40" customWidth="1"/>
     <col min="17" max="17" width="24.28515625" style="41" customWidth="1"/>
     <col min="18" max="18" width="22.28515625" style="39" customWidth="1"/>
-    <col min="19" max="19" width="13" style="40" customWidth="1"/>
+    <col min="19" max="19" width="20.42578125" style="40" customWidth="1"/>
     <col min="20" max="20" width="14.7109375" style="40" customWidth="1"/>
     <col min="21" max="21" width="12.7109375" style="40" customWidth="1"/>
     <col min="22" max="22" width="8.28515625" style="42" customWidth="1"/>
@@ -5727,9 +5727,9 @@
     <col min="31" max="31" width="12.7109375" style="40" customWidth="1"/>
     <col min="32" max="32" width="10.7109375" style="40" customWidth="1"/>
     <col min="33" max="33" width="11.85546875" style="41" customWidth="1"/>
-    <col min="34" max="34" width="10.28515625" style="3" customWidth="1"/>
+    <col min="34" max="34" width="21.85546875" style="3" customWidth="1"/>
     <col min="35" max="35" width="18.140625" style="39" customWidth="1"/>
-    <col min="36" max="36" width="27.7109375" style="40" customWidth="1"/>
+    <col min="36" max="36" width="45.7109375" style="40" customWidth="1"/>
     <col min="37" max="37" width="19.85546875" style="40" customWidth="1"/>
     <col min="38" max="38" width="20" style="40" customWidth="1"/>
     <col min="39" max="39" width="30.5703125" style="40" customWidth="1"/>
@@ -5852,10 +5852,10 @@
         <v>121</v>
       </c>
       <c r="AJ1" s="16" t="s">
+        <v>1038</v>
+      </c>
+      <c r="AK1" s="16" t="s">
         <v>65</v>
-      </c>
-      <c r="AK1" s="16" t="s">
-        <v>1032</v>
       </c>
       <c r="AL1" s="16" t="s">
         <v>66</v>
@@ -5967,7 +5967,7 @@
         <v>576</v>
       </c>
       <c r="AJ2" s="44" t="s">
-        <v>1034</v>
+        <v>1083</v>
       </c>
       <c r="AK2" s="44" t="s">
         <v>1026</v>
@@ -6080,7 +6080,7 @@
         <v>577</v>
       </c>
       <c r="AJ3" s="44" t="s">
-        <v>1035</v>
+        <v>1084</v>
       </c>
       <c r="AK3" s="44" t="s">
         <v>1027</v>
@@ -6207,7 +6207,7 @@
         <v>578</v>
       </c>
       <c r="AJ4" s="44" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="AK4" s="44" t="s">
         <v>1000</v>
@@ -6334,7 +6334,7 @@
         <v>579</v>
       </c>
       <c r="AJ5" s="44" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="AK5" s="44" t="s">
         <v>1001</v>
@@ -6461,7 +6461,7 @@
         <v>580</v>
       </c>
       <c r="AJ6" s="44" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="AK6" s="44" t="s">
         <v>1002</v>
@@ -6588,7 +6588,7 @@
         <v>581</v>
       </c>
       <c r="AJ7" s="44" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="AK7" s="44" t="s">
         <v>1003</v>
@@ -6715,7 +6715,7 @@
         <v>582</v>
       </c>
       <c r="AJ8" s="44" t="s">
-        <v>1040</v>
+        <v>1036</v>
       </c>
       <c r="AK8" s="44" t="s">
         <v>1004</v>
@@ -6828,7 +6828,7 @@
         <v>583</v>
       </c>
       <c r="AJ9" s="44" t="s">
-        <v>1041</v>
+        <v>1085</v>
       </c>
       <c r="AK9" s="44" t="s">
         <v>1028</v>
@@ -6941,7 +6941,7 @@
         <v>584</v>
       </c>
       <c r="AJ10" s="44" t="s">
-        <v>1042</v>
+        <v>1086</v>
       </c>
       <c r="AK10" s="44" t="s">
         <v>1029</v>
@@ -7054,7 +7054,7 @@
         <v>585</v>
       </c>
       <c r="AJ11" s="44" t="s">
-        <v>1043</v>
+        <v>1087</v>
       </c>
       <c r="AK11" s="44" t="s">
         <v>1030</v>
@@ -7167,7 +7167,7 @@
         <v>586</v>
       </c>
       <c r="AJ12" s="44" t="s">
-        <v>1044</v>
+        <v>1088</v>
       </c>
       <c r="AK12" s="44" t="s">
         <v>1031</v>
@@ -7633,7 +7633,7 @@
         <v>590</v>
       </c>
       <c r="AJ16" s="44" t="s">
-        <v>1048</v>
+        <v>1039</v>
       </c>
       <c r="AK16" s="44" t="s">
         <v>1005</v>
@@ -7655,7 +7655,7 @@
         <v>810</v>
       </c>
       <c r="AR16" s="44" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="AS16" s="44" t="s">
         <v>439</v>
@@ -7760,7 +7760,7 @@
         <v>591</v>
       </c>
       <c r="AJ17" s="44" t="s">
-        <v>1049</v>
+        <v>1040</v>
       </c>
       <c r="AK17" s="44" t="s">
         <v>1006</v>
@@ -7782,7 +7782,7 @@
         <v>811</v>
       </c>
       <c r="AR17" s="44" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="AS17" s="44" t="s">
         <v>439</v>
@@ -7887,7 +7887,7 @@
         <v>592</v>
       </c>
       <c r="AJ18" s="44" t="s">
-        <v>1050</v>
+        <v>1041</v>
       </c>
       <c r="AK18" s="44" t="s">
         <v>1007</v>
@@ -8014,7 +8014,7 @@
         <v>593</v>
       </c>
       <c r="AJ19" s="44" t="s">
-        <v>1051</v>
+        <v>1042</v>
       </c>
       <c r="AK19" s="44" t="s">
         <v>1008</v>
@@ -8141,7 +8141,7 @@
         <v>594</v>
       </c>
       <c r="AJ20" s="44" t="s">
-        <v>1052</v>
+        <v>1043</v>
       </c>
       <c r="AK20" s="44" t="s">
         <v>1009</v>
@@ -8267,7 +8267,7 @@
         <v>595</v>
       </c>
       <c r="AJ21" s="40" t="s">
-        <v>1053</v>
+        <v>1044</v>
       </c>
       <c r="AK21" s="44" t="s">
         <v>1010</v>
@@ -8289,7 +8289,7 @@
         <v>812</v>
       </c>
       <c r="AR21" s="44" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="AS21" s="44" t="s">
         <v>439</v>
@@ -8377,7 +8377,7 @@
         <v>596</v>
       </c>
       <c r="AJ22" s="44" t="s">
-        <v>1054</v>
+        <v>1049</v>
       </c>
       <c r="AK22" s="44" t="s">
         <v>970</v>
@@ -8487,7 +8487,7 @@
         <v>597</v>
       </c>
       <c r="AJ23" s="44" t="s">
-        <v>1055</v>
+        <v>1048</v>
       </c>
       <c r="AK23" s="44" t="s">
         <v>971</v>
@@ -8597,7 +8597,7 @@
         <v>598</v>
       </c>
       <c r="AJ24" s="44" t="s">
-        <v>1056</v>
+        <v>1050</v>
       </c>
       <c r="AK24" s="44" t="s">
         <v>972</v>
@@ -8707,7 +8707,7 @@
         <v>599</v>
       </c>
       <c r="AJ25" s="44" t="s">
-        <v>1057</v>
+        <v>1051</v>
       </c>
       <c r="AK25" s="44" t="s">
         <v>973</v>
@@ -8834,7 +8834,7 @@
         <v>600</v>
       </c>
       <c r="AJ26" s="3" t="s">
-        <v>1058</v>
+        <v>1052</v>
       </c>
       <c r="AK26" s="44" t="s">
         <v>1011</v>
@@ -8961,7 +8961,7 @@
         <v>601</v>
       </c>
       <c r="AJ27" s="44" t="s">
-        <v>1059</v>
+        <v>1053</v>
       </c>
       <c r="AK27" s="44" t="s">
         <v>1012</v>
@@ -9088,7 +9088,7 @@
         <v>602</v>
       </c>
       <c r="AJ28" s="44" t="s">
-        <v>1060</v>
+        <v>1054</v>
       </c>
       <c r="AK28" s="44" t="s">
         <v>1013</v>
@@ -9215,7 +9215,7 @@
         <v>603</v>
       </c>
       <c r="AJ29" s="44" t="s">
-        <v>1061</v>
+        <v>1055</v>
       </c>
       <c r="AK29" s="44" t="s">
         <v>1014</v>
@@ -9342,7 +9342,7 @@
         <v>604</v>
       </c>
       <c r="AJ30" s="44" t="s">
-        <v>1062</v>
+        <v>1056</v>
       </c>
       <c r="AK30" s="44" t="s">
         <v>1015</v>
@@ -9452,7 +9452,7 @@
         <v>605</v>
       </c>
       <c r="AJ31" s="44" t="s">
-        <v>1063</v>
+        <v>1082</v>
       </c>
       <c r="AK31" s="44" t="s">
         <v>974</v>
@@ -9579,7 +9579,7 @@
         <v>606</v>
       </c>
       <c r="AJ32" s="44" t="s">
-        <v>1064</v>
+        <v>1057</v>
       </c>
       <c r="AK32" s="44" t="s">
         <v>1016</v>
@@ -9706,7 +9706,7 @@
         <v>607</v>
       </c>
       <c r="AJ33" s="44" t="s">
-        <v>1065</v>
+        <v>1058</v>
       </c>
       <c r="AK33" s="44" t="s">
         <v>1017</v>
@@ -9832,7 +9832,7 @@
         <v>608</v>
       </c>
       <c r="AJ34" s="40" t="s">
-        <v>1066</v>
+        <v>1059</v>
       </c>
       <c r="AK34" s="44" t="s">
         <v>1018</v>
@@ -9959,7 +9959,7 @@
         <v>609</v>
       </c>
       <c r="AJ35" s="3" t="s">
-        <v>1067</v>
+        <v>1060</v>
       </c>
       <c r="AK35" s="44" t="s">
         <v>1019</v>
@@ -10086,7 +10086,7 @@
         <v>610</v>
       </c>
       <c r="AJ36" s="44" t="s">
-        <v>1068</v>
+        <v>1061</v>
       </c>
       <c r="AK36" s="44" t="s">
         <v>1020</v>
@@ -10213,7 +10213,7 @@
         <v>611</v>
       </c>
       <c r="AJ37" s="44" t="s">
-        <v>1069</v>
+        <v>1062</v>
       </c>
       <c r="AK37" s="44" t="s">
         <v>1021</v>
@@ -10340,7 +10340,7 @@
         <v>612</v>
       </c>
       <c r="AJ38" s="44" t="s">
-        <v>1070</v>
+        <v>1063</v>
       </c>
       <c r="AK38" s="44" t="s">
         <v>1022</v>
@@ -10467,7 +10467,7 @@
         <v>613</v>
       </c>
       <c r="AJ39" s="44" t="s">
-        <v>1071</v>
+        <v>1064</v>
       </c>
       <c r="AK39" s="44" t="s">
         <v>1023</v>
@@ -10594,7 +10594,7 @@
         <v>614</v>
       </c>
       <c r="AJ40" s="44" t="s">
-        <v>1072</v>
+        <v>1065</v>
       </c>
       <c r="AK40" s="44" t="s">
         <v>1024</v>
@@ -10616,7 +10616,7 @@
         <v>847</v>
       </c>
       <c r="AR40" s="44" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="AS40" s="44" t="s">
         <v>439</v>
@@ -10709,7 +10709,7 @@
         <v>615</v>
       </c>
       <c r="AJ41" s="44" t="s">
-        <v>1073</v>
+        <v>1066</v>
       </c>
       <c r="AK41" s="44" t="s">
         <v>975</v>
@@ -10731,7 +10731,7 @@
         <v>848</v>
       </c>
       <c r="AR41" s="44" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="AS41" s="44" t="s">
         <v>439</v>
@@ -10822,7 +10822,7 @@
         <v>616</v>
       </c>
       <c r="AJ42" s="44" t="s">
-        <v>1074</v>
+        <v>1067</v>
       </c>
       <c r="AK42" s="44" t="s">
         <v>981</v>
@@ -10935,7 +10935,7 @@
         <v>617</v>
       </c>
       <c r="AJ43" s="44" t="s">
-        <v>1075</v>
+        <v>1068</v>
       </c>
       <c r="AK43" s="44" t="s">
         <v>982</v>
@@ -11048,7 +11048,7 @@
         <v>618</v>
       </c>
       <c r="AJ44" s="44" t="s">
-        <v>1076</v>
+        <v>1069</v>
       </c>
       <c r="AK44" s="44" t="s">
         <v>983</v>
@@ -11161,7 +11161,7 @@
         <v>619</v>
       </c>
       <c r="AJ45" s="44" t="s">
-        <v>1077</v>
+        <v>1070</v>
       </c>
       <c r="AK45" s="44" t="s">
         <v>984</v>
@@ -11274,7 +11274,7 @@
         <v>620</v>
       </c>
       <c r="AJ46" s="44" t="s">
-        <v>1078</v>
+        <v>1071</v>
       </c>
       <c r="AK46" s="44" t="s">
         <v>985</v>
@@ -11387,7 +11387,7 @@
         <v>621</v>
       </c>
       <c r="AJ47" s="44" t="s">
-        <v>1079</v>
+        <v>1072</v>
       </c>
       <c r="AK47" s="44" t="s">
         <v>986</v>
@@ -11409,7 +11409,7 @@
         <v>815</v>
       </c>
       <c r="AR47" s="44" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="AS47" s="44" t="s">
         <v>439</v>
@@ -11502,7 +11502,7 @@
         <v>622</v>
       </c>
       <c r="AJ48" s="44" t="s">
-        <v>1080</v>
+        <v>1073</v>
       </c>
       <c r="AK48" s="44" t="s">
         <v>976</v>
@@ -11524,7 +11524,7 @@
         <v>816</v>
       </c>
       <c r="AR48" s="44" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="AS48" s="44" t="s">
         <v>439</v>
@@ -11617,7 +11617,7 @@
         <v>623</v>
       </c>
       <c r="AJ49" s="44" t="s">
-        <v>1081</v>
+        <v>1074</v>
       </c>
       <c r="AK49" s="44" t="s">
         <v>977</v>
@@ -11732,7 +11732,7 @@
         <v>624</v>
       </c>
       <c r="AJ50" s="44" t="s">
-        <v>1082</v>
+        <v>1075</v>
       </c>
       <c r="AK50" s="44" t="s">
         <v>978</v>
@@ -11847,7 +11847,7 @@
         <v>625</v>
       </c>
       <c r="AJ51" s="44" t="s">
-        <v>1083</v>
+        <v>1076</v>
       </c>
       <c r="AK51" s="44" t="s">
         <v>979</v>
@@ -11962,7 +11962,7 @@
         <v>626</v>
       </c>
       <c r="AJ52" s="44" t="s">
-        <v>1084</v>
+        <v>1077</v>
       </c>
       <c r="AK52" s="44" t="s">
         <v>980</v>
@@ -12096,7 +12096,7 @@
         <v>881</v>
       </c>
       <c r="AJ53" s="44" t="s">
-        <v>1085</v>
+        <v>1078</v>
       </c>
       <c r="AK53" s="44" t="s">
         <v>987</v>
@@ -12214,7 +12214,7 @@
         <v>882</v>
       </c>
       <c r="AJ54" s="44" t="s">
-        <v>1086</v>
+        <v>1079</v>
       </c>
       <c r="AK54" s="44" t="s">
         <v>988</v>
@@ -12332,7 +12332,7 @@
         <v>883</v>
       </c>
       <c r="AJ55" s="44" t="s">
-        <v>1087</v>
+        <v>1080</v>
       </c>
       <c r="AK55" s="44" t="s">
         <v>887</v>
@@ -12468,7 +12468,7 @@
         <v>884</v>
       </c>
       <c r="AJ56" s="44" t="s">
-        <v>1088</v>
+        <v>1081</v>
       </c>
       <c r="AK56" s="44" t="s">
         <v>888</v>

</xml_diff>

<commit_message>
Added new columns for easier handling of variable synonyms in Variable section.
</commit_message>
<xml_diff>
--- a/ontology_cip_2015_10_26_short.xlsx
+++ b/ontology_cip_2015_10_26_short.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="3" r:id="rId1"/>
@@ -19,14 +19,14 @@
     <sheet name="Meta2" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sweetpotato ontology'!$B$1:$AV$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sweetpotato ontology'!$B$1:$AY$52</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2363" uniqueCount="1089">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2428" uniqueCount="1104">
   <si>
     <t>List of columns in template and short description:</t>
   </si>
@@ -3311,6 +3311,51 @@
   </si>
   <si>
     <t>Number of non-commercial storage roots counting number per plot</t>
+  </si>
+  <si>
+    <t>Synonym FAO</t>
+  </si>
+  <si>
+    <t>Synonym NCSU</t>
+  </si>
+  <si>
+    <t>SCOL</t>
+  </si>
+  <si>
+    <t>RTSKN1</t>
+  </si>
+  <si>
+    <t>RTFSH1</t>
+  </si>
+  <si>
+    <t>WED1</t>
+  </si>
+  <si>
+    <t>FCOL</t>
+  </si>
+  <si>
+    <t>Synonym SASHA</t>
+  </si>
+  <si>
+    <t>ALT1</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>WED</t>
+  </si>
+  <si>
+    <t>PROTEIN</t>
+  </si>
+  <si>
+    <t>PRO</t>
+  </si>
+  <si>
+    <t>This template is a modified version of 5.0.1 intended currently for internal use at CIP (International Potato Center). Modifications include additional columns in the variable section and a modified usage of the scale category labels.</t>
+  </si>
+  <si>
+    <t>A tool is in preparation as of November, 2015 to map this file format to 5.0.1. Contact: Reinhard Simon (r.simon@cgiar.org)</t>
   </si>
 </sst>
 </file>
@@ -3410,7 +3455,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3495,6 +3540,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -3556,7 +3607,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -3694,6 +3745,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -3794,7 +3850,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1962150</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>185057</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3862,7 +3918,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>923925</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>166007</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4246,8 +4302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU125"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4265,8 +4321,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="1:47" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="P2" s="32"/>
       <c r="Y2" s="48" t="s">
         <v>216</v>
@@ -4351,14 +4406,26 @@
       </c>
     </row>
     <row r="9" spans="1:47" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
+      <c r="A9" s="63" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B9" s="64"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
       <c r="P9" s="32"/>
       <c r="AU9" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:47" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
+      <c r="A10" s="63" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B10" s="64"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
       <c r="P10" s="32"/>
       <c r="AU10" s="32">
         <v>0</v>
@@ -5683,14 +5750,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV56"/>
+  <dimension ref="A1:AY56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AJ2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="AQ2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E7" sqref="E7"/>
       <selection pane="topRight" activeCell="E7" sqref="E7"/>
       <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
-      <selection pane="bottomRight" activeCell="AJ13" sqref="AJ13"/>
+      <selection pane="bottomRight" activeCell="AL2" sqref="AL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5731,21 +5798,24 @@
     <col min="35" max="35" width="18.140625" style="39" customWidth="1"/>
     <col min="36" max="36" width="45.7109375" style="40" customWidth="1"/>
     <col min="37" max="37" width="19.85546875" style="40" customWidth="1"/>
-    <col min="38" max="38" width="20" style="40" customWidth="1"/>
-    <col min="39" max="39" width="30.5703125" style="40" customWidth="1"/>
-    <col min="40" max="40" width="12.85546875" style="40" customWidth="1"/>
-    <col min="41" max="41" width="14.7109375" style="40" customWidth="1"/>
-    <col min="42" max="42" width="11" style="40" customWidth="1"/>
-    <col min="43" max="43" width="28.28515625" style="40" customWidth="1"/>
-    <col min="44" max="44" width="16.28515625" style="40" customWidth="1"/>
-    <col min="45" max="45" width="13.7109375" style="40" customWidth="1"/>
-    <col min="46" max="46" width="17.28515625" style="40" customWidth="1"/>
-    <col min="47" max="47" width="18.42578125" style="40" customWidth="1"/>
-    <col min="48" max="48" width="12.28515625" style="41" customWidth="1"/>
-    <col min="49" max="16384" width="5" style="3"/>
+    <col min="38" max="38" width="15.7109375" style="40" customWidth="1"/>
+    <col min="39" max="39" width="13.5703125" style="40" customWidth="1"/>
+    <col min="40" max="40" width="14.42578125" style="40" customWidth="1"/>
+    <col min="41" max="41" width="20" style="40" customWidth="1"/>
+    <col min="42" max="42" width="30.5703125" style="40" customWidth="1"/>
+    <col min="43" max="43" width="12.85546875" style="40" customWidth="1"/>
+    <col min="44" max="44" width="14.7109375" style="40" customWidth="1"/>
+    <col min="45" max="45" width="11" style="40" customWidth="1"/>
+    <col min="46" max="46" width="28.28515625" style="40" customWidth="1"/>
+    <col min="47" max="47" width="16.28515625" style="40" customWidth="1"/>
+    <col min="48" max="48" width="13.7109375" style="40" customWidth="1"/>
+    <col min="49" max="49" width="17.28515625" style="40" customWidth="1"/>
+    <col min="50" max="50" width="18.42578125" style="40" customWidth="1"/>
+    <col min="51" max="51" width="12.28515625" style="41" customWidth="1"/>
+    <col min="52" max="16384" width="5" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>83</v>
       </c>
@@ -5858,40 +5928,49 @@
         <v>65</v>
       </c>
       <c r="AL1" s="16" t="s">
+        <v>1096</v>
+      </c>
+      <c r="AM1" s="16" t="s">
+        <v>1089</v>
+      </c>
+      <c r="AN1" s="16" t="s">
+        <v>1090</v>
+      </c>
+      <c r="AO1" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="AM1" s="16" t="s">
+      <c r="AP1" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="AN1" s="16" t="s">
+      <c r="AQ1" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="AO1" s="16" t="s">
+      <c r="AR1" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="AP1" s="16" t="s">
+      <c r="AS1" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="AQ1" s="16" t="s">
+      <c r="AT1" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="AR1" s="16" t="s">
+      <c r="AU1" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="AS1" s="16" t="s">
+      <c r="AV1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="AT1" s="16" t="s">
+      <c r="AW1" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="AU1" s="16" t="s">
+      <c r="AX1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="AV1" s="16" t="s">
+      <c r="AY1" s="16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:48" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="47" t="s">
         <v>627</v>
       </c>
@@ -5975,36 +6054,41 @@
       <c r="AL2" s="47" t="s">
         <v>232</v>
       </c>
-      <c r="AM2" s="44" t="s">
+      <c r="AM2" s="44"/>
+      <c r="AN2" s="44"/>
+      <c r="AO2" s="47" t="s">
+        <v>232</v>
+      </c>
+      <c r="AP2" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN2" s="44" t="s">
+      <c r="AQ2" s="44" t="s">
         <v>300</v>
       </c>
-      <c r="AO2" s="44" t="s">
+      <c r="AR2" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP2" s="44"/>
-      <c r="AQ2" s="44" t="s">
+      <c r="AS2" s="44"/>
+      <c r="AT2" s="44" t="s">
         <v>786</v>
       </c>
-      <c r="AR2" s="44" t="s">
+      <c r="AU2" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS2" s="44" t="s">
+      <c r="AV2" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT2" s="44" t="s">
+      <c r="AW2" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU2" s="51">
+      <c r="AX2" s="51">
         <v>42299</v>
       </c>
-      <c r="AV2" s="44" t="s">
+      <c r="AY2" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B3" s="47" t="s">
         <v>628</v>
       </c>
@@ -6088,36 +6172,41 @@
       <c r="AL3" s="47" t="s">
         <v>234</v>
       </c>
-      <c r="AM3" s="44" t="s">
+      <c r="AM3" s="44"/>
+      <c r="AN3" s="44"/>
+      <c r="AO3" s="47" t="s">
+        <v>234</v>
+      </c>
+      <c r="AP3" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN3" s="44" t="s">
+      <c r="AQ3" s="44" t="s">
         <v>228</v>
       </c>
-      <c r="AO3" s="44" t="s">
+      <c r="AR3" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP3" s="44"/>
-      <c r="AQ3" s="44" t="s">
+      <c r="AS3" s="44"/>
+      <c r="AT3" s="44" t="s">
         <v>787</v>
       </c>
-      <c r="AR3" s="44" t="s">
+      <c r="AU3" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS3" s="44" t="s">
+      <c r="AV3" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT3" s="44" t="s">
+      <c r="AW3" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU3" s="51">
+      <c r="AX3" s="51">
         <v>42299</v>
       </c>
-      <c r="AV3" s="44" t="s">
+      <c r="AY3" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B4" s="47" t="s">
         <v>629</v>
       </c>
@@ -6215,36 +6304,41 @@
       <c r="AL4" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="AM4" s="44" t="s">
+      <c r="AM4" s="44"/>
+      <c r="AN4" s="44"/>
+      <c r="AO4" s="47" t="s">
+        <v>235</v>
+      </c>
+      <c r="AP4" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN4" s="44" t="s">
+      <c r="AQ4" s="44" t="s">
         <v>228</v>
       </c>
-      <c r="AO4" s="44" t="s">
+      <c r="AR4" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP4" s="44"/>
-      <c r="AQ4" s="44" t="s">
+      <c r="AS4" s="44"/>
+      <c r="AT4" s="44" t="s">
         <v>788</v>
       </c>
-      <c r="AR4" s="44" t="s">
+      <c r="AU4" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS4" s="44" t="s">
+      <c r="AV4" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT4" s="44" t="s">
+      <c r="AW4" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU4" s="51">
+      <c r="AX4" s="51">
         <v>42299</v>
       </c>
-      <c r="AV4" s="44" t="s">
+      <c r="AY4" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B5" s="47" t="s">
         <v>630</v>
       </c>
@@ -6342,36 +6436,41 @@
       <c r="AL5" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="AM5" s="44" t="s">
+      <c r="AM5" s="44"/>
+      <c r="AN5" s="44"/>
+      <c r="AO5" s="47" t="s">
+        <v>236</v>
+      </c>
+      <c r="AP5" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN5" s="44" t="s">
+      <c r="AQ5" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="AO5" s="44" t="s">
+      <c r="AR5" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP5" s="44"/>
-      <c r="AQ5" s="44" t="s">
+      <c r="AS5" s="44"/>
+      <c r="AT5" s="44" t="s">
         <v>789</v>
       </c>
-      <c r="AR5" s="44" t="s">
+      <c r="AU5" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS5" s="44" t="s">
+      <c r="AV5" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT5" s="44" t="s">
+      <c r="AW5" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU5" s="51">
+      <c r="AX5" s="51">
         <v>42299</v>
       </c>
-      <c r="AV5" s="44" t="s">
+      <c r="AY5" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.2">
       <c r="B6" s="47" t="s">
         <v>631</v>
       </c>
@@ -6469,36 +6568,41 @@
       <c r="AL6" s="47" t="s">
         <v>266</v>
       </c>
-      <c r="AM6" s="44" t="s">
+      <c r="AM6" s="44"/>
+      <c r="AN6" s="44"/>
+      <c r="AO6" s="47" t="s">
+        <v>266</v>
+      </c>
+      <c r="AP6" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN6" s="44" t="s">
+      <c r="AQ6" s="44" t="s">
         <v>228</v>
       </c>
-      <c r="AO6" s="44" t="s">
+      <c r="AR6" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP6" s="44"/>
-      <c r="AQ6" s="44" t="s">
+      <c r="AS6" s="44"/>
+      <c r="AT6" s="44" t="s">
         <v>790</v>
       </c>
-      <c r="AR6" s="44" t="s">
+      <c r="AU6" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS6" s="44" t="s">
+      <c r="AV6" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT6" s="44" t="s">
+      <c r="AW6" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU6" s="51">
+      <c r="AX6" s="51">
         <v>42299</v>
       </c>
-      <c r="AV6" s="44" t="s">
+      <c r="AY6" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B7" s="47" t="s">
         <v>632</v>
       </c>
@@ -6594,38 +6698,45 @@
         <v>1003</v>
       </c>
       <c r="AL7" s="47" t="s">
+        <v>1097</v>
+      </c>
+      <c r="AM7" s="44" t="s">
+        <v>1098</v>
+      </c>
+      <c r="AN7" s="44"/>
+      <c r="AO7" s="47" t="s">
         <v>571</v>
       </c>
-      <c r="AM7" s="44" t="s">
+      <c r="AP7" s="44" t="s">
         <v>846</v>
       </c>
-      <c r="AN7" s="44" t="s">
+      <c r="AQ7" s="44" t="s">
         <v>228</v>
       </c>
-      <c r="AO7" s="44" t="s">
+      <c r="AR7" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP7" s="44"/>
-      <c r="AQ7" s="44" t="s">
+      <c r="AS7" s="44"/>
+      <c r="AT7" s="44" t="s">
         <v>791</v>
       </c>
-      <c r="AR7" s="44" t="s">
+      <c r="AU7" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS7" s="44" t="s">
+      <c r="AV7" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT7" s="44" t="s">
+      <c r="AW7" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU7" s="51">
+      <c r="AX7" s="51">
         <v>42299</v>
       </c>
-      <c r="AV7" s="44" t="s">
+      <c r="AY7" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B8" s="47" t="s">
         <v>633</v>
       </c>
@@ -6723,36 +6834,41 @@
       <c r="AL8" s="47" t="s">
         <v>237</v>
       </c>
-      <c r="AM8" s="44" t="s">
+      <c r="AM8" s="44"/>
+      <c r="AN8" s="44"/>
+      <c r="AO8" s="47" t="s">
+        <v>237</v>
+      </c>
+      <c r="AP8" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN8" s="44" t="s">
+      <c r="AQ8" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="AO8" s="44" t="s">
+      <c r="AR8" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP8" s="44"/>
-      <c r="AQ8" s="44" t="s">
+      <c r="AS8" s="44"/>
+      <c r="AT8" s="44" t="s">
         <v>792</v>
       </c>
-      <c r="AR8" s="44" t="s">
+      <c r="AU8" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS8" s="44" t="s">
+      <c r="AV8" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT8" s="44" t="s">
+      <c r="AW8" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU8" s="51">
+      <c r="AX8" s="51">
         <v>42299</v>
       </c>
-      <c r="AV8" s="44" t="s">
+      <c r="AY8" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B9" s="47" t="s">
         <v>634</v>
       </c>
@@ -6836,36 +6952,41 @@
       <c r="AL9" s="47" t="s">
         <v>239</v>
       </c>
-      <c r="AM9" s="44" t="s">
+      <c r="AM9" s="44"/>
+      <c r="AN9" s="44"/>
+      <c r="AO9" s="47" t="s">
+        <v>239</v>
+      </c>
+      <c r="AP9" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN9" s="44" t="s">
+      <c r="AQ9" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO9" s="44" t="s">
+      <c r="AR9" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP9" s="44"/>
-      <c r="AQ9" s="44" t="s">
+      <c r="AS9" s="44"/>
+      <c r="AT9" s="44" t="s">
         <v>793</v>
       </c>
-      <c r="AR9" s="44" t="s">
+      <c r="AU9" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS9" s="44" t="s">
+      <c r="AV9" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT9" s="44" t="s">
+      <c r="AW9" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU9" s="51">
+      <c r="AX9" s="51">
         <v>42299</v>
       </c>
-      <c r="AV9" s="44" t="s">
+      <c r="AY9" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B10" s="47" t="s">
         <v>635</v>
       </c>
@@ -6949,36 +7070,41 @@
       <c r="AL10" s="47" t="s">
         <v>241</v>
       </c>
-      <c r="AM10" s="44" t="s">
+      <c r="AM10" s="44"/>
+      <c r="AN10" s="44"/>
+      <c r="AO10" s="47" t="s">
+        <v>241</v>
+      </c>
+      <c r="AP10" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN10" s="44" t="s">
+      <c r="AQ10" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO10" s="44" t="s">
+      <c r="AR10" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP10" s="44"/>
-      <c r="AQ10" s="44" t="s">
+      <c r="AS10" s="44"/>
+      <c r="AT10" s="44" t="s">
         <v>794</v>
       </c>
-      <c r="AR10" s="44" t="s">
+      <c r="AU10" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS10" s="44" t="s">
+      <c r="AV10" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT10" s="44" t="s">
+      <c r="AW10" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU10" s="51">
+      <c r="AX10" s="51">
         <v>42299</v>
       </c>
-      <c r="AV10" s="44" t="s">
+      <c r="AY10" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B11" s="47" t="s">
         <v>636</v>
       </c>
@@ -7062,36 +7188,41 @@
       <c r="AL11" s="47" t="s">
         <v>242</v>
       </c>
-      <c r="AM11" s="44" t="s">
+      <c r="AM11" s="44"/>
+      <c r="AN11" s="44"/>
+      <c r="AO11" s="47" t="s">
+        <v>242</v>
+      </c>
+      <c r="AP11" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN11" s="44" t="s">
+      <c r="AQ11" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO11" s="44" t="s">
+      <c r="AR11" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP11" s="44"/>
-      <c r="AQ11" s="44" t="s">
+      <c r="AS11" s="44"/>
+      <c r="AT11" s="44" t="s">
         <v>795</v>
       </c>
-      <c r="AR11" s="44" t="s">
+      <c r="AU11" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS11" s="44" t="s">
+      <c r="AV11" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT11" s="44" t="s">
+      <c r="AW11" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU11" s="51">
+      <c r="AX11" s="51">
         <v>42299</v>
       </c>
-      <c r="AV11" s="44" t="s">
+      <c r="AY11" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B12" s="47" t="s">
         <v>637</v>
       </c>
@@ -7175,36 +7306,41 @@
       <c r="AL12" s="47" t="s">
         <v>243</v>
       </c>
-      <c r="AM12" s="44" t="s">
+      <c r="AM12" s="44"/>
+      <c r="AN12" s="44"/>
+      <c r="AO12" s="47" t="s">
+        <v>243</v>
+      </c>
+      <c r="AP12" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN12" s="44" t="s">
+      <c r="AQ12" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO12" s="44" t="s">
+      <c r="AR12" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP12" s="44"/>
-      <c r="AQ12" s="44" t="s">
+      <c r="AS12" s="44"/>
+      <c r="AT12" s="44" t="s">
         <v>796</v>
       </c>
-      <c r="AR12" s="44" t="s">
+      <c r="AU12" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS12" s="44" t="s">
+      <c r="AV12" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT12" s="44" t="s">
+      <c r="AW12" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU12" s="51">
+      <c r="AX12" s="51">
         <v>42299</v>
       </c>
-      <c r="AV12" s="44" t="s">
+      <c r="AY12" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B13" s="47" t="s">
         <v>638</v>
       </c>
@@ -7288,36 +7424,41 @@
       <c r="AL13" s="47" t="s">
         <v>246</v>
       </c>
-      <c r="AM13" s="44" t="s">
+      <c r="AM13" s="44"/>
+      <c r="AN13" s="44"/>
+      <c r="AO13" s="47" t="s">
+        <v>246</v>
+      </c>
+      <c r="AP13" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN13" s="44" t="s">
+      <c r="AQ13" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO13" s="44" t="s">
+      <c r="AR13" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP13" s="44"/>
-      <c r="AQ13" s="44" t="s">
+      <c r="AS13" s="44"/>
+      <c r="AT13" s="44" t="s">
         <v>797</v>
       </c>
-      <c r="AR13" s="44" t="s">
+      <c r="AU13" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS13" s="44" t="s">
+      <c r="AV13" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT13" s="44" t="s">
+      <c r="AW13" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU13" s="51">
+      <c r="AX13" s="51">
         <v>42299</v>
       </c>
-      <c r="AV13" s="44" t="s">
+      <c r="AY13" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B14" s="47" t="s">
         <v>639</v>
       </c>
@@ -7401,36 +7542,41 @@
       <c r="AL14" s="47" t="s">
         <v>247</v>
       </c>
-      <c r="AM14" s="44" t="s">
+      <c r="AM14" s="44"/>
+      <c r="AN14" s="44"/>
+      <c r="AO14" s="47" t="s">
+        <v>247</v>
+      </c>
+      <c r="AP14" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN14" s="44" t="s">
+      <c r="AQ14" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO14" s="44" t="s">
+      <c r="AR14" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP14" s="44"/>
-      <c r="AQ14" s="44" t="s">
+      <c r="AS14" s="44"/>
+      <c r="AT14" s="44" t="s">
         <v>798</v>
       </c>
-      <c r="AR14" s="44" t="s">
+      <c r="AU14" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS14" s="44" t="s">
+      <c r="AV14" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT14" s="44" t="s">
+      <c r="AW14" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU14" s="51">
+      <c r="AX14" s="51">
         <v>42299</v>
       </c>
-      <c r="AV14" s="44" t="s">
+      <c r="AY14" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B15" s="47" t="s">
         <v>640</v>
       </c>
@@ -7514,36 +7660,41 @@
       <c r="AL15" s="47" t="s">
         <v>249</v>
       </c>
-      <c r="AM15" s="44" t="s">
+      <c r="AM15" s="44"/>
+      <c r="AN15" s="44"/>
+      <c r="AO15" s="47" t="s">
+        <v>249</v>
+      </c>
+      <c r="AP15" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN15" s="44" t="s">
+      <c r="AQ15" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO15" s="44" t="s">
+      <c r="AR15" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP15" s="44"/>
-      <c r="AQ15" s="44" t="s">
+      <c r="AS15" s="44"/>
+      <c r="AT15" s="44" t="s">
         <v>799</v>
       </c>
-      <c r="AR15" s="44" t="s">
+      <c r="AU15" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS15" s="44" t="s">
+      <c r="AV15" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT15" s="44" t="s">
+      <c r="AW15" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU15" s="51">
+      <c r="AX15" s="51">
         <v>42299</v>
       </c>
-      <c r="AV15" s="44" t="s">
+      <c r="AY15" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B16" s="47" t="s">
         <v>641</v>
       </c>
@@ -7639,38 +7790,45 @@
         <v>1005</v>
       </c>
       <c r="AL16" s="44" t="s">
+        <v>1091</v>
+      </c>
+      <c r="AM16" s="44" t="s">
+        <v>1092</v>
+      </c>
+      <c r="AN16" s="44"/>
+      <c r="AO16" s="44" t="s">
         <v>572</v>
       </c>
-      <c r="AM16" s="44" t="s">
+      <c r="AP16" s="44" t="s">
         <v>846</v>
       </c>
-      <c r="AN16" s="44" t="s">
+      <c r="AQ16" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO16" s="44" t="s">
+      <c r="AR16" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP16" s="44"/>
-      <c r="AQ16" s="44" t="s">
+      <c r="AS16" s="44"/>
+      <c r="AT16" s="44" t="s">
         <v>810</v>
       </c>
-      <c r="AR16" s="44" t="s">
+      <c r="AU16" s="44" t="s">
         <v>1032</v>
       </c>
-      <c r="AS16" s="44" t="s">
+      <c r="AV16" s="44" t="s">
         <v>439</v>
       </c>
-      <c r="AT16" s="44" t="s">
+      <c r="AW16" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU16" s="51">
+      <c r="AX16" s="51">
         <v>42299</v>
       </c>
-      <c r="AV16" s="44" t="s">
+      <c r="AY16" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="17" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B17" s="47" t="s">
         <v>642</v>
       </c>
@@ -7766,38 +7924,45 @@
         <v>1006</v>
       </c>
       <c r="AL17" s="44" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AM17" s="44" t="s">
+        <v>1093</v>
+      </c>
+      <c r="AN17" s="44"/>
+      <c r="AO17" s="44" t="s">
         <v>573</v>
       </c>
-      <c r="AM17" s="44" t="s">
+      <c r="AP17" s="44" t="s">
         <v>846</v>
       </c>
-      <c r="AN17" s="44" t="s">
+      <c r="AQ17" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO17" s="44" t="s">
+      <c r="AR17" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP17" s="44"/>
-      <c r="AQ17" s="44" t="s">
+      <c r="AS17" s="44"/>
+      <c r="AT17" s="44" t="s">
         <v>811</v>
       </c>
-      <c r="AR17" s="44" t="s">
+      <c r="AU17" s="44" t="s">
         <v>1032</v>
       </c>
-      <c r="AS17" s="44" t="s">
+      <c r="AV17" s="44" t="s">
         <v>439</v>
       </c>
-      <c r="AT17" s="44" t="s">
+      <c r="AW17" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU17" s="51">
+      <c r="AX17" s="51">
         <v>42299</v>
       </c>
-      <c r="AV17" s="44" t="s">
+      <c r="AY17" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="18" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B18" s="47" t="s">
         <v>643</v>
       </c>
@@ -7895,36 +8060,41 @@
       <c r="AL18" s="47" t="s">
         <v>173</v>
       </c>
-      <c r="AM18" s="44" t="s">
+      <c r="AM18" s="44"/>
+      <c r="AN18" s="44"/>
+      <c r="AO18" s="47" t="s">
+        <v>173</v>
+      </c>
+      <c r="AP18" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN18" s="44" t="s">
+      <c r="AQ18" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO18" s="44" t="s">
+      <c r="AR18" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP18" s="44"/>
-      <c r="AQ18" s="44" t="s">
+      <c r="AS18" s="44"/>
+      <c r="AT18" s="44" t="s">
         <v>800</v>
       </c>
-      <c r="AR18" s="44" t="s">
+      <c r="AU18" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS18" s="44" t="s">
+      <c r="AV18" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT18" s="44" t="s">
+      <c r="AW18" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU18" s="51">
+      <c r="AX18" s="51">
         <v>42299</v>
       </c>
-      <c r="AV18" s="44" t="s">
+      <c r="AY18" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="19" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B19" s="47" t="s">
         <v>644</v>
       </c>
@@ -8022,36 +8192,41 @@
       <c r="AL19" s="47" t="s">
         <v>251</v>
       </c>
-      <c r="AM19" s="44" t="s">
+      <c r="AM19" s="44"/>
+      <c r="AN19" s="44"/>
+      <c r="AO19" s="47" t="s">
+        <v>251</v>
+      </c>
+      <c r="AP19" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN19" s="44" t="s">
+      <c r="AQ19" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO19" s="44" t="s">
+      <c r="AR19" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP19" s="44"/>
-      <c r="AQ19" s="44" t="s">
+      <c r="AS19" s="44"/>
+      <c r="AT19" s="44" t="s">
         <v>801</v>
       </c>
-      <c r="AR19" s="44" t="s">
+      <c r="AU19" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS19" s="44" t="s">
+      <c r="AV19" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT19" s="44" t="s">
+      <c r="AW19" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU19" s="51">
+      <c r="AX19" s="51">
         <v>42299</v>
       </c>
-      <c r="AV19" s="44" t="s">
+      <c r="AY19" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="20" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B20" s="47" t="s">
         <v>645</v>
       </c>
@@ -8149,36 +8324,41 @@
       <c r="AL20" s="47" t="s">
         <v>276</v>
       </c>
-      <c r="AM20" s="44" t="s">
+      <c r="AM20" s="44"/>
+      <c r="AN20" s="44"/>
+      <c r="AO20" s="47" t="s">
+        <v>276</v>
+      </c>
+      <c r="AP20" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN20" s="44" t="s">
+      <c r="AQ20" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO20" s="44" t="s">
+      <c r="AR20" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP20" s="44"/>
-      <c r="AQ20" s="44" t="s">
+      <c r="AS20" s="44"/>
+      <c r="AT20" s="44" t="s">
         <v>802</v>
       </c>
-      <c r="AR20" s="44" t="s">
+      <c r="AU20" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS20" s="44" t="s">
+      <c r="AV20" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT20" s="44" t="s">
+      <c r="AW20" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU20" s="51">
+      <c r="AX20" s="51">
         <v>42299</v>
       </c>
-      <c r="AV20" s="44" t="s">
+      <c r="AY20" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="21" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B21" s="47" t="s">
         <v>646</v>
       </c>
@@ -8273,38 +8453,45 @@
         <v>1010</v>
       </c>
       <c r="AL21" s="44" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AM21" s="44" t="s">
+        <v>1099</v>
+      </c>
+      <c r="AN21" s="44"/>
+      <c r="AO21" s="44" t="s">
         <v>574</v>
       </c>
-      <c r="AM21" s="44" t="s">
+      <c r="AP21" s="44" t="s">
         <v>846</v>
       </c>
-      <c r="AN21" s="44" t="s">
+      <c r="AQ21" s="44" t="s">
         <v>301</v>
       </c>
-      <c r="AO21" s="44" t="s">
+      <c r="AR21" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP21" s="44"/>
-      <c r="AQ21" s="44" t="s">
+      <c r="AS21" s="44"/>
+      <c r="AT21" s="44" t="s">
         <v>812</v>
       </c>
-      <c r="AR21" s="44" t="s">
+      <c r="AU21" s="44" t="s">
         <v>1032</v>
       </c>
-      <c r="AS21" s="44" t="s">
+      <c r="AV21" s="44" t="s">
         <v>439</v>
       </c>
-      <c r="AT21" s="44" t="s">
+      <c r="AW21" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU21" s="51">
+      <c r="AX21" s="51">
         <v>42299</v>
       </c>
-      <c r="AV21" s="44" t="s">
+      <c r="AY21" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="22" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B22" s="47" t="s">
         <v>647</v>
       </c>
@@ -8385,36 +8572,41 @@
       <c r="AL22" s="47" t="s">
         <v>254</v>
       </c>
-      <c r="AM22" s="44" t="s">
+      <c r="AM22" s="44"/>
+      <c r="AN22" s="44"/>
+      <c r="AO22" s="47" t="s">
+        <v>254</v>
+      </c>
+      <c r="AP22" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN22" s="44" t="s">
+      <c r="AQ22" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO22" s="44" t="s">
+      <c r="AR22" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP22" s="44"/>
-      <c r="AQ22" s="44" t="s">
+      <c r="AS22" s="44"/>
+      <c r="AT22" s="44" t="s">
         <v>803</v>
       </c>
-      <c r="AR22" s="44" t="s">
+      <c r="AU22" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS22" s="44" t="s">
+      <c r="AV22" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT22" s="44" t="s">
+      <c r="AW22" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU22" s="51">
+      <c r="AX22" s="51">
         <v>42299</v>
       </c>
-      <c r="AV22" s="44" t="s">
+      <c r="AY22" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="23" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B23" s="47" t="s">
         <v>648</v>
       </c>
@@ -8495,36 +8687,41 @@
       <c r="AL23" s="47" t="s">
         <v>261</v>
       </c>
-      <c r="AM23" s="44" t="s">
+      <c r="AM23" s="44"/>
+      <c r="AN23" s="44"/>
+      <c r="AO23" s="47" t="s">
+        <v>261</v>
+      </c>
+      <c r="AP23" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN23" s="44" t="s">
+      <c r="AQ23" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO23" s="44" t="s">
+      <c r="AR23" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP23" s="44"/>
-      <c r="AQ23" s="44" t="s">
+      <c r="AS23" s="44"/>
+      <c r="AT23" s="44" t="s">
         <v>804</v>
       </c>
-      <c r="AR23" s="44" t="s">
+      <c r="AU23" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS23" s="44" t="s">
+      <c r="AV23" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT23" s="44" t="s">
+      <c r="AW23" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU23" s="51">
+      <c r="AX23" s="51">
         <v>42299</v>
       </c>
-      <c r="AV23" s="44" t="s">
+      <c r="AY23" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="24" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B24" s="47" t="s">
         <v>649</v>
       </c>
@@ -8605,36 +8802,41 @@
       <c r="AL24" s="47" t="s">
         <v>277</v>
       </c>
-      <c r="AM24" s="44" t="s">
+      <c r="AM24" s="44"/>
+      <c r="AN24" s="44"/>
+      <c r="AO24" s="47" t="s">
+        <v>277</v>
+      </c>
+      <c r="AP24" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN24" s="44" t="s">
+      <c r="AQ24" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO24" s="44" t="s">
+      <c r="AR24" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP24" s="44"/>
-      <c r="AQ24" s="44" t="s">
+      <c r="AS24" s="44"/>
+      <c r="AT24" s="44" t="s">
         <v>765</v>
       </c>
-      <c r="AR24" s="44" t="s">
+      <c r="AU24" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS24" s="44" t="s">
+      <c r="AV24" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT24" s="44" t="s">
+      <c r="AW24" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU24" s="51">
+      <c r="AX24" s="51">
         <v>42299</v>
       </c>
-      <c r="AV24" s="44" t="s">
+      <c r="AY24" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="25" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B25" s="47" t="s">
         <v>650</v>
       </c>
@@ -8715,36 +8917,41 @@
       <c r="AL25" s="47" t="s">
         <v>278</v>
       </c>
-      <c r="AM25" s="44" t="s">
+      <c r="AM25" s="44"/>
+      <c r="AN25" s="44"/>
+      <c r="AO25" s="47" t="s">
+        <v>278</v>
+      </c>
+      <c r="AP25" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN25" s="44" t="s">
+      <c r="AQ25" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO25" s="44" t="s">
+      <c r="AR25" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP25" s="44"/>
-      <c r="AQ25" s="44" t="s">
+      <c r="AS25" s="44"/>
+      <c r="AT25" s="44" t="s">
         <v>766</v>
       </c>
-      <c r="AR25" s="44" t="s">
+      <c r="AU25" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS25" s="44" t="s">
+      <c r="AV25" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT25" s="44" t="s">
+      <c r="AW25" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU25" s="51">
+      <c r="AX25" s="51">
         <v>42299</v>
       </c>
-      <c r="AV25" s="44" t="s">
+      <c r="AY25" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="26" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B26" s="47" t="s">
         <v>651</v>
       </c>
@@ -8842,36 +9049,41 @@
       <c r="AL26" s="47" t="s">
         <v>279</v>
       </c>
-      <c r="AM26" s="44" t="s">
+      <c r="AM26" s="44"/>
+      <c r="AN26" s="44"/>
+      <c r="AO26" s="47" t="s">
+        <v>279</v>
+      </c>
+      <c r="AP26" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN26" s="44" t="s">
+      <c r="AQ26" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO26" s="44" t="s">
+      <c r="AR26" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP26" s="44"/>
-      <c r="AQ26" s="44" t="s">
+      <c r="AS26" s="44"/>
+      <c r="AT26" s="44" t="s">
         <v>805</v>
       </c>
-      <c r="AR26" s="44" t="s">
+      <c r="AU26" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS26" s="44" t="s">
+      <c r="AV26" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT26" s="44" t="s">
+      <c r="AW26" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU26" s="51">
+      <c r="AX26" s="51">
         <v>42299</v>
       </c>
-      <c r="AV26" s="44" t="s">
+      <c r="AY26" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="27" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B27" s="47" t="s">
         <v>652</v>
       </c>
@@ -8969,36 +9181,41 @@
       <c r="AL27" s="47" t="s">
         <v>280</v>
       </c>
-      <c r="AM27" s="44" t="s">
+      <c r="AM27" s="44"/>
+      <c r="AN27" s="44"/>
+      <c r="AO27" s="47" t="s">
+        <v>280</v>
+      </c>
+      <c r="AP27" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN27" s="44" t="s">
+      <c r="AQ27" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO27" s="44" t="s">
+      <c r="AR27" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP27" s="44"/>
-      <c r="AQ27" s="44" t="s">
+      <c r="AS27" s="44"/>
+      <c r="AT27" s="44" t="s">
         <v>806</v>
       </c>
-      <c r="AR27" s="44" t="s">
+      <c r="AU27" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS27" s="44" t="s">
+      <c r="AV27" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT27" s="44" t="s">
+      <c r="AW27" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU27" s="51">
+      <c r="AX27" s="51">
         <v>42299</v>
       </c>
-      <c r="AV27" s="44" t="s">
+      <c r="AY27" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="28" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B28" s="47" t="s">
         <v>653</v>
       </c>
@@ -9096,36 +9313,41 @@
       <c r="AL28" s="47" t="s">
         <v>281</v>
       </c>
-      <c r="AM28" s="44" t="s">
+      <c r="AM28" s="44"/>
+      <c r="AN28" s="44"/>
+      <c r="AO28" s="47" t="s">
+        <v>281</v>
+      </c>
+      <c r="AP28" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN28" s="44" t="s">
+      <c r="AQ28" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO28" s="44" t="s">
+      <c r="AR28" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP28" s="44"/>
-      <c r="AQ28" s="44" t="s">
+      <c r="AS28" s="44"/>
+      <c r="AT28" s="44" t="s">
         <v>807</v>
       </c>
-      <c r="AR28" s="44" t="s">
+      <c r="AU28" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS28" s="44" t="s">
+      <c r="AV28" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT28" s="44" t="s">
+      <c r="AW28" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU28" s="51">
+      <c r="AX28" s="51">
         <v>42299</v>
       </c>
-      <c r="AV28" s="44" t="s">
+      <c r="AY28" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="29" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B29" s="47" t="s">
         <v>654</v>
       </c>
@@ -9223,36 +9445,41 @@
       <c r="AL29" s="47" t="s">
         <v>282</v>
       </c>
-      <c r="AM29" s="44" t="s">
+      <c r="AM29" s="44"/>
+      <c r="AN29" s="44"/>
+      <c r="AO29" s="47" t="s">
+        <v>282</v>
+      </c>
+      <c r="AP29" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN29" s="44" t="s">
+      <c r="AQ29" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO29" s="44" t="s">
+      <c r="AR29" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP29" s="44"/>
-      <c r="AQ29" s="44" t="s">
+      <c r="AS29" s="44"/>
+      <c r="AT29" s="44" t="s">
         <v>808</v>
       </c>
-      <c r="AR29" s="44" t="s">
+      <c r="AU29" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS29" s="44" t="s">
+      <c r="AV29" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT29" s="44" t="s">
+      <c r="AW29" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU29" s="51">
+      <c r="AX29" s="51">
         <v>42299</v>
       </c>
-      <c r="AV29" s="44" t="s">
+      <c r="AY29" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="30" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B30" s="47" t="s">
         <v>655</v>
       </c>
@@ -9350,36 +9577,41 @@
       <c r="AL30" s="47" t="s">
         <v>275</v>
       </c>
-      <c r="AM30" s="44" t="s">
+      <c r="AM30" s="44"/>
+      <c r="AN30" s="44"/>
+      <c r="AO30" s="47" t="s">
+        <v>275</v>
+      </c>
+      <c r="AP30" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN30" s="44" t="s">
+      <c r="AQ30" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO30" s="44" t="s">
+      <c r="AR30" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP30" s="44"/>
-      <c r="AQ30" s="44" t="s">
+      <c r="AS30" s="44"/>
+      <c r="AT30" s="44" t="s">
         <v>809</v>
       </c>
-      <c r="AR30" s="44" t="s">
+      <c r="AU30" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS30" s="44" t="s">
+      <c r="AV30" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT30" s="44" t="s">
+      <c r="AW30" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU30" s="51">
+      <c r="AX30" s="51">
         <v>42299</v>
       </c>
-      <c r="AV30" s="44" t="s">
+      <c r="AY30" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="31" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B31" s="47" t="s">
         <v>656</v>
       </c>
@@ -9460,36 +9692,41 @@
       <c r="AL31" s="47" t="s">
         <v>274</v>
       </c>
-      <c r="AM31" s="44" t="s">
+      <c r="AM31" s="44"/>
+      <c r="AN31" s="44"/>
+      <c r="AO31" s="47" t="s">
+        <v>274</v>
+      </c>
+      <c r="AP31" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN31" s="44" t="s">
+      <c r="AQ31" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO31" s="44" t="s">
+      <c r="AR31" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP31" s="44"/>
-      <c r="AQ31" s="44" t="s">
+      <c r="AS31" s="44"/>
+      <c r="AT31" s="44" t="s">
         <v>767</v>
       </c>
-      <c r="AR31" s="44" t="s">
+      <c r="AU31" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS31" s="44" t="s">
+      <c r="AV31" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT31" s="44" t="s">
+      <c r="AW31" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU31" s="51">
+      <c r="AX31" s="51">
         <v>42299</v>
       </c>
-      <c r="AV31" s="44" t="s">
+      <c r="AY31" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="32" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B32" s="47" t="s">
         <v>657</v>
       </c>
@@ -9587,36 +9824,41 @@
       <c r="AL32" s="47" t="s">
         <v>267</v>
       </c>
-      <c r="AM32" s="44" t="s">
+      <c r="AM32" s="44"/>
+      <c r="AN32" s="44"/>
+      <c r="AO32" s="47" t="s">
+        <v>267</v>
+      </c>
+      <c r="AP32" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN32" s="44" t="s">
+      <c r="AQ32" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="AO32" s="44" t="s">
+      <c r="AR32" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP32" s="44"/>
-      <c r="AQ32" s="44" t="s">
+      <c r="AS32" s="44"/>
+      <c r="AT32" s="44" t="s">
         <v>768</v>
       </c>
-      <c r="AR32" s="44" t="s">
+      <c r="AU32" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS32" s="44" t="s">
+      <c r="AV32" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT32" s="44" t="s">
+      <c r="AW32" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU32" s="51">
+      <c r="AX32" s="51">
         <v>42299</v>
       </c>
-      <c r="AV32" s="44" t="s">
+      <c r="AY32" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="33" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B33" s="47" t="s">
         <v>658</v>
       </c>
@@ -9714,36 +9956,41 @@
       <c r="AL33" s="47" t="s">
         <v>272</v>
       </c>
-      <c r="AM33" s="44" t="s">
+      <c r="AM33" s="44"/>
+      <c r="AN33" s="44"/>
+      <c r="AO33" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="AP33" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN33" s="44" t="s">
+      <c r="AQ33" s="44" t="s">
         <v>301</v>
       </c>
-      <c r="AO33" s="44" t="s">
+      <c r="AR33" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP33" s="44"/>
-      <c r="AQ33" s="44" t="s">
+      <c r="AS33" s="44"/>
+      <c r="AT33" s="44" t="s">
         <v>769</v>
       </c>
-      <c r="AR33" s="44" t="s">
+      <c r="AU33" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS33" s="44" t="s">
+      <c r="AV33" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT33" s="44" t="s">
+      <c r="AW33" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU33" s="51">
+      <c r="AX33" s="51">
         <v>42299</v>
       </c>
-      <c r="AV33" s="44" t="s">
+      <c r="AY33" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="34" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B34" s="47" t="s">
         <v>659</v>
       </c>
@@ -9840,36 +10087,41 @@
       <c r="AL34" s="58" t="s">
         <v>273</v>
       </c>
-      <c r="AM34" s="44" t="s">
+      <c r="AM34" s="44"/>
+      <c r="AN34" s="44"/>
+      <c r="AO34" s="58" t="s">
+        <v>273</v>
+      </c>
+      <c r="AP34" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN34" s="44" t="s">
+      <c r="AQ34" s="44" t="s">
         <v>301</v>
       </c>
-      <c r="AO34" s="44" t="s">
+      <c r="AR34" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP34" s="44"/>
-      <c r="AQ34" s="44" t="s">
+      <c r="AS34" s="44"/>
+      <c r="AT34" s="44" t="s">
         <v>770</v>
       </c>
-      <c r="AR34" s="44" t="s">
+      <c r="AU34" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS34" s="44" t="s">
+      <c r="AV34" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT34" s="44" t="s">
+      <c r="AW34" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU34" s="51">
+      <c r="AX34" s="51">
         <v>42299</v>
       </c>
-      <c r="AV34" s="44" t="s">
+      <c r="AY34" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="35" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B35" s="47" t="s">
         <v>660</v>
       </c>
@@ -9967,36 +10219,41 @@
       <c r="AL35" s="47" t="s">
         <v>283</v>
       </c>
-      <c r="AM35" s="44" t="s">
+      <c r="AM35" s="44"/>
+      <c r="AN35" s="44"/>
+      <c r="AO35" s="47" t="s">
+        <v>283</v>
+      </c>
+      <c r="AP35" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN35" s="44" t="s">
+      <c r="AQ35" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO35" s="44" t="s">
+      <c r="AR35" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP35" s="44"/>
-      <c r="AQ35" s="44" t="s">
+      <c r="AS35" s="44"/>
+      <c r="AT35" s="44" t="s">
         <v>771</v>
       </c>
-      <c r="AR35" s="44" t="s">
+      <c r="AU35" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS35" s="44" t="s">
+      <c r="AV35" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT35" s="44" t="s">
+      <c r="AW35" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU35" s="51">
+      <c r="AX35" s="51">
         <v>42299</v>
       </c>
-      <c r="AV35" s="44" t="s">
+      <c r="AY35" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="36" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B36" s="47" t="s">
         <v>661</v>
       </c>
@@ -10094,36 +10351,41 @@
       <c r="AL36" s="47" t="s">
         <v>284</v>
       </c>
-      <c r="AM36" s="44" t="s">
+      <c r="AM36" s="44"/>
+      <c r="AN36" s="44"/>
+      <c r="AO36" s="47" t="s">
+        <v>284</v>
+      </c>
+      <c r="AP36" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN36" s="44" t="s">
+      <c r="AQ36" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO36" s="44" t="s">
+      <c r="AR36" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP36" s="44"/>
-      <c r="AQ36" s="44" t="s">
+      <c r="AS36" s="44"/>
+      <c r="AT36" s="44" t="s">
         <v>772</v>
       </c>
-      <c r="AR36" s="44" t="s">
+      <c r="AU36" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS36" s="44" t="s">
+      <c r="AV36" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT36" s="44" t="s">
+      <c r="AW36" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU36" s="51">
+      <c r="AX36" s="51">
         <v>42299</v>
       </c>
-      <c r="AV36" s="44" t="s">
+      <c r="AY36" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="37" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B37" s="47" t="s">
         <v>662</v>
       </c>
@@ -10221,36 +10483,41 @@
       <c r="AL37" s="47" t="s">
         <v>285</v>
       </c>
-      <c r="AM37" s="44" t="s">
+      <c r="AM37" s="44"/>
+      <c r="AN37" s="44"/>
+      <c r="AO37" s="47" t="s">
+        <v>285</v>
+      </c>
+      <c r="AP37" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN37" s="44" t="s">
+      <c r="AQ37" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO37" s="44" t="s">
+      <c r="AR37" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP37" s="44"/>
-      <c r="AQ37" s="44" t="s">
+      <c r="AS37" s="44"/>
+      <c r="AT37" s="44" t="s">
         <v>773</v>
       </c>
-      <c r="AR37" s="44" t="s">
+      <c r="AU37" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS37" s="44" t="s">
+      <c r="AV37" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT37" s="44" t="s">
+      <c r="AW37" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU37" s="51">
+      <c r="AX37" s="51">
         <v>42299</v>
       </c>
-      <c r="AV37" s="44" t="s">
+      <c r="AY37" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="38" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B38" s="47" t="s">
         <v>663</v>
       </c>
@@ -10348,36 +10615,41 @@
       <c r="AL38" s="47" t="s">
         <v>286</v>
       </c>
-      <c r="AM38" s="44" t="s">
+      <c r="AM38" s="44"/>
+      <c r="AN38" s="44"/>
+      <c r="AO38" s="47" t="s">
+        <v>286</v>
+      </c>
+      <c r="AP38" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN38" s="44" t="s">
+      <c r="AQ38" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO38" s="44" t="s">
+      <c r="AR38" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP38" s="44"/>
-      <c r="AQ38" s="44" t="s">
+      <c r="AS38" s="44"/>
+      <c r="AT38" s="44" t="s">
         <v>774</v>
       </c>
-      <c r="AR38" s="44" t="s">
+      <c r="AU38" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS38" s="44" t="s">
+      <c r="AV38" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT38" s="44" t="s">
+      <c r="AW38" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU38" s="51">
+      <c r="AX38" s="51">
         <v>42299</v>
       </c>
-      <c r="AV38" s="44" t="s">
+      <c r="AY38" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="39" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B39" s="47" t="s">
         <v>664</v>
       </c>
@@ -10475,36 +10747,41 @@
       <c r="AL39" s="47" t="s">
         <v>287</v>
       </c>
-      <c r="AM39" s="44" t="s">
+      <c r="AM39" s="44"/>
+      <c r="AN39" s="44"/>
+      <c r="AO39" s="47" t="s">
+        <v>287</v>
+      </c>
+      <c r="AP39" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN39" s="44" t="s">
+      <c r="AQ39" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO39" s="44" t="s">
+      <c r="AR39" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP39" s="44"/>
-      <c r="AQ39" s="44" t="s">
+      <c r="AS39" s="44"/>
+      <c r="AT39" s="44" t="s">
         <v>775</v>
       </c>
-      <c r="AR39" s="44" t="s">
+      <c r="AU39" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS39" s="44" t="s">
+      <c r="AV39" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT39" s="44" t="s">
+      <c r="AW39" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU39" s="51">
+      <c r="AX39" s="51">
         <v>42299</v>
       </c>
-      <c r="AV39" s="44" t="s">
+      <c r="AY39" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="40" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B40" s="47" t="s">
         <v>665</v>
       </c>
@@ -10602,36 +10879,41 @@
       <c r="AL40" s="44" t="s">
         <v>288</v>
       </c>
-      <c r="AM40" s="44" t="s">
+      <c r="AM40" s="44"/>
+      <c r="AN40" s="44"/>
+      <c r="AO40" s="44" t="s">
+        <v>288</v>
+      </c>
+      <c r="AP40" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN40" s="44" t="s">
+      <c r="AQ40" s="44" t="s">
         <v>299</v>
       </c>
-      <c r="AO40" s="44" t="s">
+      <c r="AR40" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP40" s="44"/>
-      <c r="AQ40" s="44" t="s">
+      <c r="AS40" s="44"/>
+      <c r="AT40" s="44" t="s">
         <v>847</v>
       </c>
-      <c r="AR40" s="44" t="s">
+      <c r="AU40" s="44" t="s">
         <v>1032</v>
       </c>
-      <c r="AS40" s="44" t="s">
+      <c r="AV40" s="44" t="s">
         <v>439</v>
       </c>
-      <c r="AT40" s="44" t="s">
+      <c r="AW40" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU40" s="51">
+      <c r="AX40" s="51">
         <v>42299</v>
       </c>
-      <c r="AV40" s="44" t="s">
+      <c r="AY40" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="41" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B41" s="47" t="s">
         <v>666</v>
       </c>
@@ -10715,38 +10997,45 @@
         <v>975</v>
       </c>
       <c r="AL41" s="44" t="s">
+        <v>1100</v>
+      </c>
+      <c r="AM41" s="44" t="s">
+        <v>1101</v>
+      </c>
+      <c r="AN41" s="44"/>
+      <c r="AO41" s="44" t="s">
         <v>575</v>
       </c>
-      <c r="AM41" s="44" t="s">
+      <c r="AP41" s="44" t="s">
         <v>846</v>
       </c>
-      <c r="AN41" s="44" t="s">
+      <c r="AQ41" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO41" s="44" t="s">
+      <c r="AR41" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP41" s="44"/>
-      <c r="AQ41" s="44" t="s">
+      <c r="AS41" s="44"/>
+      <c r="AT41" s="44" t="s">
         <v>848</v>
       </c>
-      <c r="AR41" s="44" t="s">
+      <c r="AU41" s="44" t="s">
         <v>1032</v>
       </c>
-      <c r="AS41" s="44" t="s">
+      <c r="AV41" s="44" t="s">
         <v>439</v>
       </c>
-      <c r="AT41" s="44" t="s">
+      <c r="AW41" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU41" s="51">
+      <c r="AX41" s="51">
         <v>42299</v>
       </c>
-      <c r="AV41" s="44" t="s">
+      <c r="AY41" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="42" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B42" s="47" t="s">
         <v>667</v>
       </c>
@@ -10830,36 +11119,41 @@
       <c r="AL42" s="44" t="s">
         <v>291</v>
       </c>
-      <c r="AM42" s="44" t="s">
+      <c r="AM42" s="44"/>
+      <c r="AN42" s="44"/>
+      <c r="AO42" s="44" t="s">
+        <v>291</v>
+      </c>
+      <c r="AP42" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN42" s="44" t="s">
+      <c r="AQ42" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO42" s="44" t="s">
+      <c r="AR42" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP42" s="44"/>
-      <c r="AQ42" s="44" t="s">
+      <c r="AS42" s="44"/>
+      <c r="AT42" s="44" t="s">
         <v>776</v>
       </c>
-      <c r="AR42" s="44" t="s">
+      <c r="AU42" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS42" s="44" t="s">
+      <c r="AV42" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT42" s="44" t="s">
+      <c r="AW42" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU42" s="51">
+      <c r="AX42" s="51">
         <v>42299</v>
       </c>
-      <c r="AV42" s="44" t="s">
+      <c r="AY42" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="43" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B43" s="47" t="s">
         <v>668</v>
       </c>
@@ -10943,36 +11237,41 @@
       <c r="AL43" s="44" t="s">
         <v>292</v>
       </c>
-      <c r="AM43" s="44" t="s">
+      <c r="AM43" s="44"/>
+      <c r="AN43" s="44"/>
+      <c r="AO43" s="44" t="s">
+        <v>292</v>
+      </c>
+      <c r="AP43" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN43" s="44" t="s">
+      <c r="AQ43" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO43" s="44" t="s">
+      <c r="AR43" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP43" s="44"/>
-      <c r="AQ43" s="44" t="s">
+      <c r="AS43" s="44"/>
+      <c r="AT43" s="44" t="s">
         <v>777</v>
       </c>
-      <c r="AR43" s="44" t="s">
+      <c r="AU43" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS43" s="44" t="s">
+      <c r="AV43" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT43" s="44" t="s">
+      <c r="AW43" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU43" s="51">
+      <c r="AX43" s="51">
         <v>42299</v>
       </c>
-      <c r="AV43" s="44" t="s">
+      <c r="AY43" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="44" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B44" s="47" t="s">
         <v>669</v>
       </c>
@@ -11056,36 +11355,41 @@
       <c r="AL44" s="47" t="s">
         <v>293</v>
       </c>
-      <c r="AM44" s="44" t="s">
+      <c r="AM44" s="44"/>
+      <c r="AN44" s="44"/>
+      <c r="AO44" s="47" t="s">
+        <v>293</v>
+      </c>
+      <c r="AP44" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN44" s="44" t="s">
+      <c r="AQ44" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO44" s="44" t="s">
+      <c r="AR44" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP44" s="44"/>
-      <c r="AQ44" s="44" t="s">
+      <c r="AS44" s="44"/>
+      <c r="AT44" s="44" t="s">
         <v>778</v>
       </c>
-      <c r="AR44" s="44" t="s">
+      <c r="AU44" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS44" s="44" t="s">
+      <c r="AV44" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT44" s="44" t="s">
+      <c r="AW44" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU44" s="51">
+      <c r="AX44" s="51">
         <v>42299</v>
       </c>
-      <c r="AV44" s="44" t="s">
+      <c r="AY44" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="45" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B45" s="47" t="s">
         <v>670</v>
       </c>
@@ -11169,36 +11473,41 @@
       <c r="AL45" s="47" t="s">
         <v>294</v>
       </c>
-      <c r="AM45" s="44" t="s">
+      <c r="AM45" s="44"/>
+      <c r="AN45" s="44"/>
+      <c r="AO45" s="47" t="s">
+        <v>294</v>
+      </c>
+      <c r="AP45" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN45" s="44" t="s">
+      <c r="AQ45" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO45" s="44" t="s">
+      <c r="AR45" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP45" s="44"/>
-      <c r="AQ45" s="44" t="s">
+      <c r="AS45" s="44"/>
+      <c r="AT45" s="44" t="s">
         <v>779</v>
       </c>
-      <c r="AR45" s="44" t="s">
+      <c r="AU45" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS45" s="44" t="s">
+      <c r="AV45" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT45" s="44" t="s">
+      <c r="AW45" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU45" s="51">
+      <c r="AX45" s="51">
         <v>42299</v>
       </c>
-      <c r="AV45" s="44" t="s">
+      <c r="AY45" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="46" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B46" s="47" t="s">
         <v>671</v>
       </c>
@@ -11282,36 +11591,41 @@
       <c r="AL46" s="47" t="s">
         <v>174</v>
       </c>
-      <c r="AM46" s="44" t="s">
+      <c r="AM46" s="44"/>
+      <c r="AN46" s="44"/>
+      <c r="AO46" s="47" t="s">
+        <v>174</v>
+      </c>
+      <c r="AP46" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN46" s="44" t="s">
+      <c r="AQ46" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO46" s="44" t="s">
+      <c r="AR46" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP46" s="44"/>
-      <c r="AQ46" s="44" t="s">
+      <c r="AS46" s="44"/>
+      <c r="AT46" s="44" t="s">
         <v>780</v>
       </c>
-      <c r="AR46" s="44" t="s">
+      <c r="AU46" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS46" s="44" t="s">
+      <c r="AV46" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT46" s="44" t="s">
+      <c r="AW46" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU46" s="51">
+      <c r="AX46" s="51">
         <v>42299</v>
       </c>
-      <c r="AV46" s="44" t="s">
+      <c r="AY46" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="47" spans="2:48" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B47" s="47" t="s">
         <v>672</v>
       </c>
@@ -11395,36 +11709,41 @@
       <c r="AL47" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="AM47" s="44" t="s">
+      <c r="AM47" s="44"/>
+      <c r="AN47" s="44"/>
+      <c r="AO47" s="44" t="s">
+        <v>175</v>
+      </c>
+      <c r="AP47" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN47" s="44" t="s">
+      <c r="AQ47" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO47" s="44" t="s">
+      <c r="AR47" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP47" s="44"/>
-      <c r="AQ47" s="44" t="s">
+      <c r="AS47" s="44"/>
+      <c r="AT47" s="44" t="s">
         <v>815</v>
       </c>
-      <c r="AR47" s="44" t="s">
+      <c r="AU47" s="44" t="s">
         <v>1032</v>
       </c>
-      <c r="AS47" s="44" t="s">
+      <c r="AV47" s="44" t="s">
         <v>439</v>
       </c>
-      <c r="AT47" s="44" t="s">
+      <c r="AW47" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU47" s="51">
+      <c r="AX47" s="51">
         <v>42299</v>
       </c>
-      <c r="AV47" s="44" t="s">
+      <c r="AY47" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="48" spans="2:48" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="47" t="s">
         <v>673</v>
       </c>
@@ -11510,36 +11829,41 @@
       <c r="AL48" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="AM48" s="44" t="s">
+      <c r="AM48" s="44"/>
+      <c r="AN48" s="44"/>
+      <c r="AO48" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="AP48" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN48" s="44" t="s">
+      <c r="AQ48" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO48" s="44" t="s">
+      <c r="AR48" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP48" s="44"/>
-      <c r="AQ48" s="44" t="s">
+      <c r="AS48" s="44"/>
+      <c r="AT48" s="44" t="s">
         <v>816</v>
       </c>
-      <c r="AR48" s="44" t="s">
+      <c r="AU48" s="44" t="s">
         <v>1032</v>
       </c>
-      <c r="AS48" s="44" t="s">
+      <c r="AV48" s="44" t="s">
         <v>439</v>
       </c>
-      <c r="AT48" s="44" t="s">
+      <c r="AW48" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU48" s="51">
+      <c r="AX48" s="51">
         <v>42299</v>
       </c>
-      <c r="AV48" s="44" t="s">
+      <c r="AY48" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="49" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B49" s="47" t="s">
         <v>674</v>
       </c>
@@ -11625,36 +11949,41 @@
       <c r="AL49" s="47" t="s">
         <v>177</v>
       </c>
-      <c r="AM49" s="44" t="s">
+      <c r="AM49" s="44"/>
+      <c r="AN49" s="44"/>
+      <c r="AO49" s="47" t="s">
+        <v>177</v>
+      </c>
+      <c r="AP49" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN49" s="44" t="s">
+      <c r="AQ49" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO49" s="44" t="s">
+      <c r="AR49" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP49" s="44"/>
-      <c r="AQ49" s="44" t="s">
+      <c r="AS49" s="44"/>
+      <c r="AT49" s="44" t="s">
         <v>781</v>
       </c>
-      <c r="AR49" s="44" t="s">
+      <c r="AU49" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS49" s="44" t="s">
+      <c r="AV49" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT49" s="44" t="s">
+      <c r="AW49" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU49" s="51">
+      <c r="AX49" s="51">
         <v>42299</v>
       </c>
-      <c r="AV49" s="44" t="s">
+      <c r="AY49" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="50" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B50" s="47" t="s">
         <v>675</v>
       </c>
@@ -11740,36 +12069,41 @@
       <c r="AL50" s="47" t="s">
         <v>178</v>
       </c>
-      <c r="AM50" s="44" t="s">
+      <c r="AM50" s="44"/>
+      <c r="AN50" s="44"/>
+      <c r="AO50" s="47" t="s">
+        <v>178</v>
+      </c>
+      <c r="AP50" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN50" s="44" t="s">
+      <c r="AQ50" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO50" s="44" t="s">
+      <c r="AR50" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP50" s="44"/>
-      <c r="AQ50" s="44" t="s">
+      <c r="AS50" s="44"/>
+      <c r="AT50" s="44" t="s">
         <v>782</v>
       </c>
-      <c r="AR50" s="44" t="s">
+      <c r="AU50" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS50" s="44" t="s">
+      <c r="AV50" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT50" s="44" t="s">
+      <c r="AW50" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU50" s="51">
+      <c r="AX50" s="51">
         <v>42299</v>
       </c>
-      <c r="AV50" s="44" t="s">
+      <c r="AY50" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="51" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B51" s="47" t="s">
         <v>676</v>
       </c>
@@ -11855,36 +12189,41 @@
       <c r="AL51" s="47" t="s">
         <v>179</v>
       </c>
-      <c r="AM51" s="44" t="s">
+      <c r="AM51" s="44"/>
+      <c r="AN51" s="44"/>
+      <c r="AO51" s="47" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP51" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN51" s="44" t="s">
+      <c r="AQ51" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO51" s="44" t="s">
+      <c r="AR51" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP51" s="44"/>
-      <c r="AQ51" s="44" t="s">
+      <c r="AS51" s="44"/>
+      <c r="AT51" s="44" t="s">
         <v>783</v>
       </c>
-      <c r="AR51" s="44" t="s">
+      <c r="AU51" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS51" s="44" t="s">
+      <c r="AV51" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT51" s="44" t="s">
+      <c r="AW51" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU51" s="51">
+      <c r="AX51" s="51">
         <v>42299</v>
       </c>
-      <c r="AV51" s="44" t="s">
+      <c r="AY51" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="52" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:51" x14ac:dyDescent="0.25">
       <c r="B52" s="47" t="s">
         <v>677</v>
       </c>
@@ -11970,36 +12309,41 @@
       <c r="AL52" s="47" t="s">
         <v>180</v>
       </c>
-      <c r="AM52" s="44" t="s">
+      <c r="AM52" s="44"/>
+      <c r="AN52" s="44"/>
+      <c r="AO52" s="47" t="s">
+        <v>180</v>
+      </c>
+      <c r="AP52" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN52" s="44" t="s">
+      <c r="AQ52" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO52" s="44" t="s">
+      <c r="AR52" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP52" s="44"/>
-      <c r="AQ52" s="44" t="s">
+      <c r="AS52" s="44"/>
+      <c r="AT52" s="44" t="s">
         <v>784</v>
       </c>
-      <c r="AR52" s="44" t="s">
+      <c r="AU52" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS52" s="44" t="s">
+      <c r="AV52" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT52" s="44" t="s">
+      <c r="AW52" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU52" s="51">
+      <c r="AX52" s="51">
         <v>42299</v>
       </c>
-      <c r="AV52" s="44" t="s">
+      <c r="AY52" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="53" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A53" s="44"/>
       <c r="B53" s="47" t="s">
         <v>861</v>
@@ -12104,36 +12448,41 @@
       <c r="AL53" s="44" t="s">
         <v>865</v>
       </c>
-      <c r="AM53" s="44" t="s">
+      <c r="AM53" s="44"/>
+      <c r="AN53" s="44"/>
+      <c r="AO53" s="44" t="s">
+        <v>865</v>
+      </c>
+      <c r="AP53" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN53" s="44" t="s">
+      <c r="AQ53" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO53" s="44" t="s">
+      <c r="AR53" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP53" s="44"/>
-      <c r="AQ53" s="44" t="s">
+      <c r="AS53" s="44"/>
+      <c r="AT53" s="44" t="s">
         <v>809</v>
       </c>
-      <c r="AR53" s="44" t="s">
+      <c r="AU53" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS53" s="44" t="s">
+      <c r="AV53" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT53" s="44" t="s">
+      <c r="AW53" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU53" s="51">
+      <c r="AX53" s="51">
         <v>42299</v>
       </c>
-      <c r="AV53" s="44" t="s">
+      <c r="AY53" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="54" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A54" s="44"/>
       <c r="B54" s="47" t="s">
         <v>862</v>
@@ -12222,36 +12571,41 @@
       <c r="AL54" s="44" t="s">
         <v>854</v>
       </c>
-      <c r="AM54" s="44" t="s">
+      <c r="AM54" s="44"/>
+      <c r="AN54" s="44"/>
+      <c r="AO54" s="44" t="s">
+        <v>854</v>
+      </c>
+      <c r="AP54" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN54" s="44" t="s">
+      <c r="AQ54" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO54" s="44" t="s">
+      <c r="AR54" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP54" s="44"/>
-      <c r="AQ54" s="44" t="s">
+      <c r="AS54" s="44"/>
+      <c r="AT54" s="44" t="s">
         <v>866</v>
       </c>
-      <c r="AR54" s="44" t="s">
+      <c r="AU54" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS54" s="44" t="s">
+      <c r="AV54" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT54" s="44" t="s">
+      <c r="AW54" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU54" s="51">
+      <c r="AX54" s="51">
         <v>42299</v>
       </c>
-      <c r="AV54" s="44" t="s">
+      <c r="AY54" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="55" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A55" s="44"/>
       <c r="B55" s="47" t="s">
         <v>863</v>
@@ -12340,36 +12694,41 @@
       <c r="AL55" s="44" t="s">
         <v>891</v>
       </c>
-      <c r="AM55" s="44" t="s">
+      <c r="AM55" s="44"/>
+      <c r="AN55" s="44"/>
+      <c r="AO55" s="44" t="s">
+        <v>891</v>
+      </c>
+      <c r="AP55" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN55" s="44" t="s">
+      <c r="AQ55" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO55" s="44" t="s">
+      <c r="AR55" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP55" s="44"/>
-      <c r="AQ55" s="44" t="s">
+      <c r="AS55" s="44"/>
+      <c r="AT55" s="44" t="s">
         <v>867</v>
       </c>
-      <c r="AR55" s="44" t="s">
+      <c r="AU55" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS55" s="44" t="s">
+      <c r="AV55" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT55" s="44" t="s">
+      <c r="AW55" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU55" s="51">
+      <c r="AX55" s="51">
         <v>42299</v>
       </c>
-      <c r="AV55" s="44" t="s">
+      <c r="AY55" s="44" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="56" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A56" s="44"/>
       <c r="B56" s="47" t="s">
         <v>864</v>
@@ -12476,42 +12835,48 @@
       <c r="AL56" s="44" t="s">
         <v>857</v>
       </c>
-      <c r="AM56" s="44" t="s">
+      <c r="AM56" s="44"/>
+      <c r="AN56" s="44"/>
+      <c r="AO56" s="44" t="s">
+        <v>857</v>
+      </c>
+      <c r="AP56" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AN56" s="44" t="s">
+      <c r="AQ56" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="AO56" s="44" t="s">
+      <c r="AR56" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="AP56" s="44"/>
-      <c r="AQ56" s="44" t="s">
+      <c r="AS56" s="44"/>
+      <c r="AT56" s="44" t="s">
         <v>868</v>
       </c>
-      <c r="AR56" s="44" t="s">
+      <c r="AU56" s="44" t="s">
         <v>1025</v>
       </c>
-      <c r="AS56" s="44" t="s">
+      <c r="AV56" s="44" t="s">
         <v>438</v>
       </c>
-      <c r="AT56" s="44" t="s">
+      <c r="AW56" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="AU56" s="51">
+      <c r="AX56" s="51">
         <v>42299</v>
       </c>
-      <c r="AV56" s="44" t="s">
+      <c r="AY56" s="44" t="s">
         <v>570</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="AL34" r:id="rId1" display="WED@"/>
+    <hyperlink ref="AO34" r:id="rId1" display="WED@"/>
+    <hyperlink ref="AL34" r:id="rId2" display="WED@"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId3"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>